<commit_message>
deleted some .DS_Store files
Accounts update

Financial planning update (Lisi Kredit)
</commit_message>
<xml_diff>
--- a/Planning/overview_planning_25.xlsx
+++ b/Planning/overview_planning_25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6a293577490f170/Financials/Planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernd\financials\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="548" documentId="13_ncr:1_{249F5035-DC70-D24C-AB9D-A4CF2488C603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C129EAB1-60C3-2349-AE5B-F4892E6CC29F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855658F5-FD5A-48D5-989A-827A7B7A88A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview25" sheetId="1" r:id="rId1"/>
@@ -957,7 +957,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1092,6 +1092,10 @@
     <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="18" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="10" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1099,17 +1103,6 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="10" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="10" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent 1 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1145,10 +1138,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1324,11 +1313,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMC176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="3" customWidth="1"/>
@@ -1349,14 +1338,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="20">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-    </row>
-    <row r="3" spans="2:14" ht="15">
+      <c r="C1" s="108"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+    </row>
+    <row r="3" spans="2:14" ht="14">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1368,10 +1357,10 @@
       </c>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="2:14" ht="15">
+    <row r="4" spans="2:14" ht="14">
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="2:14" ht="15">
+    <row r="5" spans="2:14" ht="14">
       <c r="B5" s="12" t="s">
         <v>3</v>
       </c>
@@ -1409,7 +1398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="15">
+    <row r="6" spans="2:14" ht="14">
       <c r="B6" s="16">
         <v>45658</v>
       </c>
@@ -1431,7 +1420,7 @@
       <c r="M6" s="21"/>
       <c r="N6" s="22"/>
     </row>
-    <row r="7" spans="2:14" ht="15">
+    <row r="7" spans="2:14" ht="14">
       <c r="B7" s="23">
         <v>45658</v>
       </c>
@@ -1447,7 +1436,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="2:14" ht="15">
+    <row r="8" spans="2:14" ht="14">
       <c r="B8" s="23">
         <v>45662</v>
       </c>
@@ -1462,7 +1451,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="28"/>
     </row>
-    <row r="9" spans="2:14" ht="15">
+    <row r="9" spans="2:14" ht="14">
       <c r="B9" s="23">
         <v>45667</v>
       </c>
@@ -1483,7 +1472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15">
+    <row r="10" spans="2:14" ht="14">
       <c r="B10" s="23">
         <v>45677</v>
       </c>
@@ -1503,7 +1492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="15">
+    <row r="11" spans="2:14" ht="14">
       <c r="B11" s="26">
         <v>45692</v>
       </c>
@@ -1525,7 +1514,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="15">
+    <row r="12" spans="2:14" ht="14">
       <c r="B12" s="26">
         <v>45695</v>
       </c>
@@ -1538,7 +1527,7 @@
       <c r="H12" s="23"/>
       <c r="N12" s="28"/>
     </row>
-    <row r="13" spans="2:14" ht="15">
+    <row r="13" spans="2:14" ht="14">
       <c r="B13" s="16">
         <v>45695</v>
       </c>
@@ -1552,7 +1541,7 @@
       <c r="H13" s="23"/>
       <c r="N13" s="28"/>
     </row>
-    <row r="14" spans="2:14" ht="15">
+    <row r="14" spans="2:14" ht="14">
       <c r="B14" s="26">
         <v>45695</v>
       </c>
@@ -1565,7 +1554,7 @@
       <c r="H14" s="23"/>
       <c r="N14" s="28"/>
     </row>
-    <row r="15" spans="2:14" ht="15">
+    <row r="15" spans="2:14" ht="14">
       <c r="B15" s="26">
         <v>45696</v>
       </c>
@@ -1580,7 +1569,7 @@
       <c r="M15" s="4"/>
       <c r="N15" s="28"/>
     </row>
-    <row r="16" spans="2:14" ht="15">
+    <row r="16" spans="2:14" ht="14">
       <c r="B16" s="26">
         <v>45698</v>
       </c>
@@ -1595,7 +1584,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="28"/>
     </row>
-    <row r="17" spans="2:14" ht="15">
+    <row r="17" spans="2:14" ht="14">
       <c r="B17" s="23" t="s">
         <v>19</v>
       </c>
@@ -1608,7 +1597,7 @@
       <c r="H17" s="23"/>
       <c r="N17" s="28"/>
     </row>
-    <row r="18" spans="2:14" ht="15">
+    <row r="18" spans="2:14" ht="14">
       <c r="B18" s="23" t="s">
         <v>19</v>
       </c>
@@ -1623,7 +1612,7 @@
       <c r="M18" s="4"/>
       <c r="N18" s="28"/>
     </row>
-    <row r="19" spans="2:14" ht="15">
+    <row r="19" spans="2:14" ht="14">
       <c r="B19" s="23" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +1627,7 @@
       <c r="M19" s="4"/>
       <c r="N19" s="28"/>
     </row>
-    <row r="20" spans="2:14" ht="15">
+    <row r="20" spans="2:14" ht="14">
       <c r="B20" s="16" t="s">
         <v>22</v>
       </c>
@@ -1654,7 +1643,7 @@
       <c r="M20" s="4"/>
       <c r="N20" s="28"/>
     </row>
-    <row r="21" spans="2:14" ht="15">
+    <row r="21" spans="2:14" ht="14">
       <c r="B21" s="23" t="s">
         <v>24</v>
       </c>
@@ -1670,7 +1659,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="28"/>
     </row>
-    <row r="22" spans="2:14" ht="15">
+    <row r="22" spans="2:14" ht="14">
       <c r="B22" s="23" t="s">
         <v>26</v>
       </c>
@@ -1686,7 +1675,7 @@
       <c r="M22" s="4"/>
       <c r="N22" s="28"/>
     </row>
-    <row r="23" spans="2:14" ht="15">
+    <row r="23" spans="2:14" ht="14">
       <c r="B23" s="23" t="s">
         <v>28</v>
       </c>
@@ -1702,7 +1691,7 @@
       <c r="M23" s="4"/>
       <c r="N23" s="28"/>
     </row>
-    <row r="24" spans="2:14" ht="15">
+    <row r="24" spans="2:14" ht="14">
       <c r="B24" s="23" t="s">
         <v>30</v>
       </c>
@@ -1716,7 +1705,7 @@
       <c r="H24" s="23"/>
       <c r="N24" s="28"/>
     </row>
-    <row r="25" spans="2:14" ht="15">
+    <row r="25" spans="2:14" ht="14">
       <c r="B25" s="23" t="s">
         <v>32</v>
       </c>
@@ -1732,7 +1721,7 @@
       <c r="M25" s="4"/>
       <c r="N25" s="27"/>
     </row>
-    <row r="26" spans="2:14" ht="15">
+    <row r="26" spans="2:14" ht="14">
       <c r="B26" s="26">
         <v>45719</v>
       </c>
@@ -1754,7 +1743,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:14" ht="15">
+    <row r="27" spans="2:14" ht="14">
       <c r="B27" s="26">
         <v>45721</v>
       </c>
@@ -1769,7 +1758,7 @@
       <c r="M27" s="4"/>
       <c r="N27" s="28"/>
     </row>
-    <row r="28" spans="2:14" ht="15">
+    <row r="28" spans="2:14" ht="14">
       <c r="B28" s="26">
         <v>45724</v>
       </c>
@@ -1784,7 +1773,7 @@
       <c r="M28" s="4"/>
       <c r="N28" s="27"/>
     </row>
-    <row r="29" spans="2:14" ht="15">
+    <row r="29" spans="2:14" ht="14">
       <c r="B29" s="26">
         <v>45724</v>
       </c>
@@ -1799,7 +1788,7 @@
       <c r="M29" s="4"/>
       <c r="N29" s="27"/>
     </row>
-    <row r="30" spans="2:14" ht="15">
+    <row r="30" spans="2:14" ht="14">
       <c r="B30" s="26">
         <v>45724</v>
       </c>
@@ -1815,7 +1804,7 @@
       <c r="M30" s="4"/>
       <c r="N30" s="27"/>
     </row>
-    <row r="31" spans="2:14" ht="15">
+    <row r="31" spans="2:14" ht="14">
       <c r="B31" s="26">
         <v>45724</v>
       </c>
@@ -1830,7 +1819,7 @@
       <c r="M31" s="4"/>
       <c r="N31" s="27"/>
     </row>
-    <row r="32" spans="2:14" ht="15">
+    <row r="32" spans="2:14" ht="14">
       <c r="B32" s="26">
         <v>45729</v>
       </c>
@@ -1845,7 +1834,7 @@
       <c r="M32" s="4"/>
       <c r="N32" s="27"/>
     </row>
-    <row r="33" spans="2:14" ht="15">
+    <row r="33" spans="2:14" ht="14">
       <c r="B33" s="26">
         <v>45730</v>
       </c>
@@ -1860,7 +1849,7 @@
       <c r="M33" s="4"/>
       <c r="N33" s="27"/>
     </row>
-    <row r="34" spans="2:14" ht="15">
+    <row r="34" spans="2:14" ht="14">
       <c r="B34" s="26">
         <v>45731</v>
       </c>
@@ -1873,7 +1862,7 @@
       <c r="H34" s="23"/>
       <c r="N34" s="28"/>
     </row>
-    <row r="35" spans="2:14" ht="15">
+    <row r="35" spans="2:14" ht="14">
       <c r="B35" s="26">
         <v>45731</v>
       </c>
@@ -1886,7 +1875,7 @@
       <c r="H35" s="23"/>
       <c r="N35" s="28"/>
     </row>
-    <row r="36" spans="2:14" ht="15">
+    <row r="36" spans="2:14" ht="14">
       <c r="B36" s="26">
         <v>45732</v>
       </c>
@@ -1899,7 +1888,7 @@
       <c r="H36" s="23"/>
       <c r="N36" s="28"/>
     </row>
-    <row r="37" spans="2:14" ht="15">
+    <row r="37" spans="2:14" ht="14">
       <c r="B37" s="16">
         <v>45732</v>
       </c>
@@ -1915,7 +1904,7 @@
       <c r="M37" s="11"/>
       <c r="N37" s="27"/>
     </row>
-    <row r="38" spans="2:14" ht="15">
+    <row r="38" spans="2:14" ht="14">
       <c r="B38" s="26">
         <v>45733</v>
       </c>
@@ -1928,7 +1917,7 @@
       <c r="H38" s="23"/>
       <c r="N38" s="28"/>
     </row>
-    <row r="39" spans="2:14" ht="15">
+    <row r="39" spans="2:14" ht="14">
       <c r="B39" s="26">
         <v>45747</v>
       </c>
@@ -1951,7 +1940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="2:14" ht="15">
+    <row r="40" spans="2:14" ht="14">
       <c r="B40" s="20">
         <v>45748</v>
       </c>
@@ -2035,7 +2024,7 @@
       <c r="M43" s="11"/>
       <c r="N43" s="27"/>
     </row>
-    <row r="44" spans="2:14" ht="15">
+    <row r="44" spans="2:14" ht="14">
       <c r="B44" s="26">
         <v>45758</v>
       </c>
@@ -2049,7 +2038,7 @@
       <c r="H44" s="23"/>
       <c r="N44" s="28"/>
     </row>
-    <row r="45" spans="2:14" ht="15">
+    <row r="45" spans="2:14" ht="14">
       <c r="B45" s="26">
         <v>45762</v>
       </c>
@@ -2062,7 +2051,7 @@
       <c r="H45" s="23"/>
       <c r="N45" s="28"/>
     </row>
-    <row r="46" spans="2:14" ht="15">
+    <row r="46" spans="2:14" ht="14">
       <c r="B46" s="20">
         <v>45755</v>
       </c>
@@ -2078,7 +2067,7 @@
       <c r="M46" s="11"/>
       <c r="N46" s="27"/>
     </row>
-    <row r="47" spans="2:14" ht="15">
+    <row r="47" spans="2:14" ht="14">
       <c r="B47" s="26">
         <v>45769</v>
       </c>
@@ -2094,7 +2083,7 @@
       <c r="M47" s="11"/>
       <c r="N47" s="27"/>
     </row>
-    <row r="48" spans="2:14" ht="15">
+    <row r="48" spans="2:14" ht="14">
       <c r="B48" s="26">
         <v>45779</v>
       </c>
@@ -2115,7 +2104,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="15">
+    <row r="49" spans="2:14" ht="14">
       <c r="B49" s="26">
         <v>45779</v>
       </c>
@@ -2131,7 +2120,7 @@
       <c r="M49" s="11"/>
       <c r="N49" s="27"/>
     </row>
-    <row r="50" spans="2:14" ht="15">
+    <row r="50" spans="2:14" ht="14">
       <c r="B50" s="26">
         <v>45779</v>
       </c>
@@ -2147,7 +2136,7 @@
       <c r="M50" s="11"/>
       <c r="N50" s="27"/>
     </row>
-    <row r="51" spans="2:14" ht="15">
+    <row r="51" spans="2:14" ht="14">
       <c r="B51" s="20">
         <v>45779</v>
       </c>
@@ -2161,7 +2150,7 @@
       <c r="H51" s="23"/>
       <c r="N51" s="28"/>
     </row>
-    <row r="52" spans="2:14" ht="15">
+    <row r="52" spans="2:14" ht="14">
       <c r="B52" s="26">
         <v>45784</v>
       </c>
@@ -2174,7 +2163,7 @@
       <c r="H52" s="23"/>
       <c r="N52" s="28"/>
     </row>
-    <row r="53" spans="2:14" ht="15">
+    <row r="53" spans="2:14" ht="14">
       <c r="B53" s="26">
         <v>45784</v>
       </c>
@@ -2188,7 +2177,7 @@
       <c r="H53" s="23"/>
       <c r="N53" s="28"/>
     </row>
-    <row r="54" spans="2:14" ht="15">
+    <row r="54" spans="2:14" ht="14">
       <c r="B54" s="26">
         <v>45785</v>
       </c>
@@ -2201,7 +2190,7 @@
       <c r="H54" s="23"/>
       <c r="N54" s="28"/>
     </row>
-    <row r="55" spans="2:14" ht="15">
+    <row r="55" spans="2:14" ht="14">
       <c r="B55" s="26">
         <v>45786</v>
       </c>
@@ -2221,7 +2210,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="15">
+    <row r="56" spans="2:14" ht="14">
       <c r="B56" s="26">
         <v>45786</v>
       </c>
@@ -2234,7 +2223,7 @@
       <c r="H56" s="23"/>
       <c r="N56" s="28"/>
     </row>
-    <row r="57" spans="2:14" ht="15">
+    <row r="57" spans="2:14" ht="14">
       <c r="B57" s="26">
         <v>45790</v>
       </c>
@@ -2247,7 +2236,7 @@
       <c r="H57" s="23"/>
       <c r="N57" s="28"/>
     </row>
-    <row r="58" spans="2:14" ht="15">
+    <row r="58" spans="2:14" ht="14">
       <c r="B58" s="26">
         <v>45798</v>
       </c>
@@ -2260,7 +2249,7 @@
       <c r="H58" s="23"/>
       <c r="N58" s="28"/>
     </row>
-    <row r="59" spans="2:14" ht="15">
+    <row r="59" spans="2:14" ht="14">
       <c r="B59" s="26">
         <v>45798</v>
       </c>
@@ -2273,7 +2262,7 @@
       <c r="H59" s="23"/>
       <c r="N59" s="28"/>
     </row>
-    <row r="60" spans="2:14" ht="15">
+    <row r="60" spans="2:14" ht="14">
       <c r="B60" s="26">
         <v>45798</v>
       </c>
@@ -2286,7 +2275,7 @@
       <c r="H60" s="89"/>
       <c r="N60" s="92"/>
     </row>
-    <row r="61" spans="2:14" ht="15">
+    <row r="61" spans="2:14" ht="14">
       <c r="B61" s="26">
         <v>45798</v>
       </c>
@@ -2299,7 +2288,7 @@
       <c r="H61" s="89"/>
       <c r="N61" s="92"/>
     </row>
-    <row r="62" spans="2:14" ht="15">
+    <row r="62" spans="2:14" ht="14">
       <c r="B62" s="26">
         <v>45799</v>
       </c>
@@ -2314,7 +2303,7 @@
       <c r="M62" s="4"/>
       <c r="N62" s="93"/>
     </row>
-    <row r="63" spans="2:14" ht="15">
+    <row r="63" spans="2:14" ht="14">
       <c r="B63" s="20">
         <v>45799</v>
       </c>
@@ -2330,7 +2319,7 @@
       <c r="M63" s="4"/>
       <c r="N63" s="92"/>
     </row>
-    <row r="64" spans="2:14" ht="15">
+    <row r="64" spans="2:14" ht="14">
       <c r="B64" s="26">
         <v>45805</v>
       </c>
@@ -2343,7 +2332,7 @@
       <c r="H64" s="89"/>
       <c r="N64" s="92"/>
     </row>
-    <row r="65" spans="2:14" ht="15">
+    <row r="65" spans="2:14" ht="14">
       <c r="B65" s="26">
         <v>45807</v>
       </c>
@@ -2358,7 +2347,7 @@
       <c r="M65" s="4"/>
       <c r="N65" s="93"/>
     </row>
-    <row r="66" spans="2:14" ht="15">
+    <row r="66" spans="2:14" ht="14">
       <c r="B66" s="26">
         <v>45814</v>
       </c>
@@ -2380,7 +2369,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="2:14" ht="15">
+    <row r="67" spans="2:14" ht="14">
       <c r="B67" s="26">
         <v>45816</v>
       </c>
@@ -2404,7 +2393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="2:14" ht="15">
+    <row r="68" spans="2:14" ht="14">
       <c r="B68" s="26">
         <v>45820</v>
       </c>
@@ -2419,7 +2408,7 @@
       <c r="M68" s="4"/>
       <c r="N68" s="93"/>
     </row>
-    <row r="69" spans="2:14" ht="15">
+    <row r="69" spans="2:14" ht="14">
       <c r="B69" s="26">
         <v>45820</v>
       </c>
@@ -2434,7 +2423,7 @@
       <c r="M69" s="4"/>
       <c r="N69" s="93"/>
     </row>
-    <row r="70" spans="2:14" ht="15">
+    <row r="70" spans="2:14" ht="14">
       <c r="B70" s="20">
         <v>45820</v>
       </c>
@@ -2450,7 +2439,7 @@
       <c r="M70" s="4"/>
       <c r="N70" s="93"/>
     </row>
-    <row r="71" spans="2:14" ht="15">
+    <row r="71" spans="2:14" ht="14">
       <c r="B71" s="26">
         <v>45830</v>
       </c>
@@ -2465,7 +2454,7 @@
       <c r="M71" s="4"/>
       <c r="N71" s="93"/>
     </row>
-    <row r="72" spans="2:14" ht="15">
+    <row r="72" spans="2:14" ht="14">
       <c r="B72" s="26">
         <v>45831</v>
       </c>
@@ -2483,7 +2472,7 @@
       <c r="M72"/>
       <c r="N72" s="94"/>
     </row>
-    <row r="73" spans="2:14" ht="15">
+    <row r="73" spans="2:14" ht="14">
       <c r="B73" s="26">
         <v>45835</v>
       </c>
@@ -2501,7 +2490,7 @@
       <c r="M73"/>
       <c r="N73" s="94"/>
     </row>
-    <row r="74" spans="2:14" ht="15">
+    <row r="74" spans="2:14" ht="14">
       <c r="B74" s="26">
         <v>45838</v>
       </c>
@@ -2522,7 +2511,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="2:14" ht="15">
+    <row r="75" spans="2:14" ht="14">
       <c r="B75" s="26">
         <v>45838</v>
       </c>
@@ -2546,7 +2535,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="2:14" ht="15">
+    <row r="76" spans="2:14" ht="14">
       <c r="B76" s="26">
         <v>45840</v>
       </c>
@@ -2559,7 +2548,7 @@
       <c r="H76" s="89"/>
       <c r="N76" s="92"/>
     </row>
-    <row r="77" spans="2:14" ht="15">
+    <row r="77" spans="2:14" ht="14">
       <c r="B77" s="26">
         <v>45841</v>
       </c>
@@ -2572,7 +2561,7 @@
       <c r="H77" s="89"/>
       <c r="N77" s="92"/>
     </row>
-    <row r="78" spans="2:14" ht="15">
+    <row r="78" spans="2:14" ht="14">
       <c r="B78" s="26">
         <v>45845</v>
       </c>
@@ -2587,7 +2576,7 @@
       <c r="M78" s="11"/>
       <c r="N78" s="93"/>
     </row>
-    <row r="79" spans="2:14" ht="15">
+    <row r="79" spans="2:14" ht="14">
       <c r="B79" s="26">
         <v>45849</v>
       </c>
@@ -2603,7 +2592,7 @@
       <c r="M79" s="11"/>
       <c r="N79" s="93"/>
     </row>
-    <row r="80" spans="2:14" ht="15">
+    <row r="80" spans="2:14" ht="14">
       <c r="B80" s="26">
         <v>45849</v>
       </c>
@@ -2625,7 +2614,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="2:14" ht="15">
+    <row r="81" spans="2:14" ht="14">
       <c r="B81" s="26">
         <v>45853</v>
       </c>
@@ -2645,7 +2634,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="2:14" ht="15">
+    <row r="82" spans="2:14" ht="14">
       <c r="B82" s="26">
         <v>45854</v>
       </c>
@@ -2665,7 +2654,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="2:14" ht="15">
+    <row r="83" spans="2:14" ht="14">
       <c r="B83" s="20">
         <v>45854</v>
       </c>
@@ -2689,7 +2678,7 @@
       <c r="M83" s="29"/>
       <c r="N83" s="22"/>
     </row>
-    <row r="84" spans="2:14" ht="15">
+    <row r="84" spans="2:14" ht="14">
       <c r="B84" s="26">
         <v>45857</v>
       </c>
@@ -2704,7 +2693,7 @@
       <c r="M84" s="4"/>
       <c r="N84" s="27"/>
     </row>
-    <row r="85" spans="2:14" ht="15">
+    <row r="85" spans="2:14" ht="14">
       <c r="B85" s="26">
         <v>45861</v>
       </c>
@@ -2719,7 +2708,7 @@
       <c r="M85" s="4"/>
       <c r="N85" s="27"/>
     </row>
-    <row r="86" spans="2:14" ht="15">
+    <row r="86" spans="2:14" ht="14">
       <c r="B86" s="26">
         <v>45864</v>
       </c>
@@ -2740,7 +2729,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="87" spans="2:14" ht="15">
+    <row r="87" spans="2:14" ht="14">
       <c r="B87" s="26">
         <v>45868</v>
       </c>
@@ -2762,7 +2751,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="88" spans="2:14" ht="15">
+    <row r="88" spans="2:14" ht="14">
       <c r="B88" s="26">
         <v>45869</v>
       </c>
@@ -2777,7 +2766,7 @@
       <c r="M88" s="4"/>
       <c r="N88" s="93"/>
     </row>
-    <row r="89" spans="2:14" ht="15">
+    <row r="89" spans="2:14" ht="14">
       <c r="B89" s="26">
         <v>45871</v>
       </c>
@@ -2792,7 +2781,7 @@
       <c r="M89" s="4"/>
       <c r="N89" s="93"/>
     </row>
-    <row r="90" spans="2:14" ht="15">
+    <row r="90" spans="2:14" ht="14">
       <c r="B90" s="26">
         <v>45871</v>
       </c>
@@ -2807,7 +2796,7 @@
       <c r="M90" s="4"/>
       <c r="N90" s="93"/>
     </row>
-    <row r="91" spans="2:14" ht="15">
+    <row r="91" spans="2:14" ht="14">
       <c r="B91" s="20">
         <v>45871</v>
       </c>
@@ -2821,73 +2810,54 @@
       <c r="H91" s="89"/>
       <c r="N91" s="92"/>
     </row>
-    <row r="92" spans="2:14" ht="15">
+    <row r="92" spans="2:14" ht="14">
       <c r="B92" s="26">
         <v>45892</v>
       </c>
-      <c r="C92" s="107"/>
-      <c r="D92" s="114"/>
-      <c r="E92" s="114">
+      <c r="E92" s="4">
         <v>-882</v>
       </c>
-      <c r="F92" s="115" t="s">
+      <c r="F92" s="93" t="s">
         <v>161</v>
       </c>
       <c r="H92" s="89"/>
-      <c r="I92" s="108"/>
-      <c r="J92" s="108"/>
-      <c r="K92" s="108"/>
-      <c r="L92" s="109"/>
-      <c r="M92" s="109"/>
       <c r="N92" s="92"/>
     </row>
-    <row r="93" spans="2:14" ht="15">
+    <row r="93" spans="2:14" ht="14">
       <c r="B93" s="26">
         <v>45892</v>
       </c>
-      <c r="C93" s="107"/>
-      <c r="D93" s="114"/>
-      <c r="E93" s="114">
+      <c r="E93" s="4">
         <v>-243</v>
       </c>
-      <c r="F93" s="115" t="s">
+      <c r="F93" s="93" t="s">
         <v>162</v>
       </c>
       <c r="H93" s="89"/>
-      <c r="I93" s="108"/>
-      <c r="J93" s="108"/>
-      <c r="K93" s="108"/>
-      <c r="L93" s="109"/>
-      <c r="M93" s="109"/>
       <c r="N93" s="92"/>
     </row>
-    <row r="94" spans="2:14" ht="15">
+    <row r="94" spans="2:14" ht="14">
       <c r="B94" s="26">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="C94" s="1"/>
-      <c r="D94" s="116"/>
-      <c r="E94" s="114">
-        <v>-600</v>
+      <c r="D94" s="106"/>
+      <c r="E94" s="4">
+        <v>-640</v>
       </c>
       <c r="F94" s="93" t="s">
         <v>80</v>
       </c>
       <c r="H94" s="89"/>
-      <c r="I94" s="108"/>
-      <c r="J94" s="108"/>
-      <c r="K94" s="108"/>
-      <c r="L94" s="109"/>
-      <c r="M94" s="109"/>
       <c r="N94" s="92"/>
     </row>
-    <row r="95" spans="2:14" ht="15">
+    <row r="95" spans="2:14" ht="14">
       <c r="B95" s="26">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="C95" s="1"/>
-      <c r="D95" s="116"/>
-      <c r="E95" s="114">
+      <c r="D95" s="106"/>
+      <c r="E95" s="4">
         <v>-2000</v>
       </c>
       <c r="F95" s="93" t="s">
@@ -2896,61 +2866,47 @@
       <c r="H95" s="90">
         <v>45895</v>
       </c>
-      <c r="I95" s="108"/>
-      <c r="J95" s="108">
+      <c r="J95" s="4">
         <v>17600</v>
       </c>
-      <c r="K95" s="108"/>
-      <c r="L95" s="108"/>
-      <c r="M95" s="108"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
       <c r="N95" s="92" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="2:14" ht="15">
+    <row r="96" spans="2:14" ht="14">
       <c r="B96" s="20">
-        <v>45894</v>
+        <v>45893</v>
       </c>
       <c r="C96" s="18">
         <f>SUM(C91:E95)</f>
-        <v>30110.520000000004</v>
-      </c>
-      <c r="D96" s="110"/>
-      <c r="E96" s="110"/>
-      <c r="F96" s="117"/>
+        <v>30070.520000000004</v>
+      </c>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="107"/>
       <c r="H96" s="89"/>
-      <c r="I96" s="108"/>
-      <c r="J96" s="108"/>
-      <c r="K96" s="108"/>
-      <c r="L96" s="109"/>
-      <c r="M96" s="109"/>
       <c r="N96" s="92"/>
     </row>
-    <row r="97" spans="2:14" ht="15">
+    <row r="97" spans="2:14" ht="14">
       <c r="B97" s="26">
         <v>45895</v>
       </c>
-      <c r="D97" s="108"/>
-      <c r="E97" s="108">
+      <c r="E97" s="4">
         <v>-300</v>
       </c>
       <c r="F97" s="93" t="s">
         <v>159</v>
       </c>
       <c r="H97" s="89"/>
-      <c r="I97" s="108"/>
-      <c r="J97" s="108"/>
-      <c r="K97" s="108"/>
-      <c r="L97" s="109"/>
-      <c r="M97" s="109"/>
       <c r="N97" s="92"/>
     </row>
-    <row r="98" spans="2:14" ht="15">
+    <row r="98" spans="2:14" ht="14">
       <c r="B98" s="26">
         <v>45901</v>
       </c>
-      <c r="D98" s="108"/>
-      <c r="E98" s="108">
+      <c r="E98" s="4">
         <v>-5700</v>
       </c>
       <c r="F98" s="93" t="s">
@@ -2959,23 +2915,19 @@
       <c r="H98" s="90">
         <v>45901</v>
       </c>
-      <c r="I98" s="108"/>
-      <c r="J98" s="108"/>
-      <c r="K98" s="108"/>
-      <c r="L98" s="108">
+      <c r="L98" s="4">
         <v>-12000</v>
       </c>
-      <c r="M98" s="108"/>
+      <c r="M98" s="4"/>
       <c r="N98" s="92" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="2:14" ht="15">
+    <row r="99" spans="2:14" ht="14">
       <c r="B99" s="26">
         <v>45901</v>
       </c>
-      <c r="D99" s="108"/>
-      <c r="E99" s="108">
+      <c r="E99" s="4">
         <v>-2500</v>
       </c>
       <c r="F99" s="93" t="s">
@@ -2984,64 +2936,51 @@
       <c r="H99" s="90">
         <v>45930</v>
       </c>
-      <c r="I99" s="108"/>
-      <c r="J99" s="108"/>
-      <c r="K99" s="108">
+      <c r="K99" s="4">
         <f>-3*CostBlocks25!$C$24-K80</f>
         <v>-371</v>
       </c>
-      <c r="L99" s="108"/>
-      <c r="M99" s="108"/>
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
       <c r="N99" s="92" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="2:14" ht="15">
+    <row r="100" spans="2:14" ht="14">
       <c r="B100" s="26">
         <v>45901</v>
       </c>
-      <c r="D100" s="108">
+      <c r="D100" s="4">
         <v>12000</v>
       </c>
-      <c r="E100" s="108"/>
       <c r="F100" s="92" t="s">
         <v>8</v>
       </c>
       <c r="H100" s="89"/>
-      <c r="I100" s="108"/>
-      <c r="J100" s="108"/>
-      <c r="K100" s="108"/>
-      <c r="L100" s="109"/>
-      <c r="M100" s="109"/>
       <c r="N100" s="92"/>
     </row>
-    <row r="101" spans="2:14" ht="15">
+    <row r="101" spans="2:14" ht="14">
       <c r="B101" s="26">
         <v>45930</v>
       </c>
-      <c r="D101" s="108">
+      <c r="D101" s="4">
         <v>150</v>
       </c>
-      <c r="E101" s="108"/>
       <c r="F101" s="92" t="s">
         <v>160</v>
       </c>
       <c r="H101" s="90"/>
-      <c r="I101" s="108"/>
-      <c r="J101" s="108"/>
-      <c r="K101" s="108"/>
-      <c r="L101" s="108"/>
-      <c r="M101" s="108"/>
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
       <c r="N101" s="92"/>
     </row>
-    <row r="102" spans="2:14" ht="15">
+    <row r="102" spans="2:14" ht="14">
       <c r="B102" s="26">
         <v>45930</v>
       </c>
-      <c r="D102" s="108"/>
-      <c r="E102" s="108">
+      <c r="E102" s="4">
         <f>-CostBlocks25!$L$15-E67-E80/2-E81-E77-E85-E79-E84-E86-E88/2-E94/2</f>
-        <v>-1695.3200000000002</v>
+        <v>-1675.3200000000002</v>
       </c>
       <c r="F102" s="92" t="s">
         <v>152</v>
@@ -3049,25 +2988,20 @@
       <c r="H102" s="90">
         <v>45958</v>
       </c>
-      <c r="I102" s="108"/>
-      <c r="J102" s="108">
+      <c r="J102" s="4">
         <v>12000</v>
       </c>
-      <c r="K102" s="108"/>
-      <c r="L102" s="109"/>
-      <c r="M102" s="109"/>
       <c r="N102" s="92" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="103" spans="2:14" ht="15">
+    <row r="103" spans="2:14" ht="14">
       <c r="B103" s="26">
         <v>45930</v>
       </c>
-      <c r="D103" s="108"/>
-      <c r="E103" s="108">
+      <c r="E103" s="4">
         <f>-3*CostBlocks25!$C$19-E80/2-E88/2-E94/2</f>
-        <v>-865</v>
+        <v>-845</v>
       </c>
       <c r="F103" s="92" t="s">
         <v>84</v>
@@ -3075,18 +3009,14 @@
       <c r="H103" s="90">
         <v>45960</v>
       </c>
-      <c r="I103" s="108"/>
-      <c r="J103" s="108"/>
-      <c r="K103" s="108"/>
-      <c r="L103" s="108">
+      <c r="L103" s="4">
         <v>-10000</v>
       </c>
-      <c r="M103" s="109"/>
       <c r="N103" s="92" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="2:14" ht="15">
+    <row r="104" spans="2:14" ht="14">
       <c r="B104" s="20">
         <v>45931</v>
       </c>
@@ -3097,20 +3027,20 @@
       <c r="D104" s="18"/>
       <c r="E104" s="18"/>
       <c r="F104" s="22"/>
-      <c r="H104" s="113">
+      <c r="H104" s="105">
         <v>45962</v>
       </c>
-      <c r="I104" s="110">
+      <c r="I104" s="18">
         <f>SUM(I83:M103)</f>
         <v>7464.8499999999985</v>
       </c>
-      <c r="J104" s="110"/>
-      <c r="K104" s="110"/>
-      <c r="L104" s="111"/>
-      <c r="M104" s="111"/>
-      <c r="N104" s="112"/>
-    </row>
-    <row r="105" spans="2:14" ht="15">
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="29"/>
+      <c r="M104" s="29"/>
+      <c r="N104" s="104"/>
+    </row>
+    <row r="105" spans="2:14" ht="14">
       <c r="B105" s="26">
         <v>45938</v>
       </c>
@@ -3121,14 +3051,9 @@
         <v>146</v>
       </c>
       <c r="H105" s="89"/>
-      <c r="I105" s="108"/>
-      <c r="J105" s="108"/>
-      <c r="K105" s="108"/>
-      <c r="L105" s="109"/>
-      <c r="M105" s="109"/>
       <c r="N105" s="92"/>
     </row>
-    <row r="106" spans="2:14" ht="15">
+    <row r="106" spans="2:14" ht="14">
       <c r="B106" s="26">
         <v>45960</v>
       </c>
@@ -3137,14 +3062,9 @@
       </c>
       <c r="F106" s="28"/>
       <c r="H106" s="89"/>
-      <c r="I106" s="108"/>
-      <c r="J106" s="108"/>
-      <c r="K106" s="108"/>
-      <c r="L106" s="109"/>
-      <c r="M106" s="109"/>
       <c r="N106" s="92"/>
     </row>
-    <row r="107" spans="2:14" ht="15">
+    <row r="107" spans="2:14" ht="14">
       <c r="B107" s="26">
         <v>45960</v>
       </c>
@@ -3157,18 +3077,16 @@
       <c r="H107" s="90">
         <v>46011</v>
       </c>
-      <c r="I107" s="108"/>
-      <c r="J107" s="108">
+      <c r="J107" s="4">
         <v>12000</v>
       </c>
-      <c r="K107" s="108"/>
-      <c r="L107" s="108"/>
-      <c r="M107" s="108"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
       <c r="N107" s="93" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="2:14" ht="15">
+    <row r="108" spans="2:14" ht="14">
       <c r="B108" s="26">
         <v>45966</v>
       </c>
@@ -3181,18 +3099,15 @@
       <c r="H108" s="90">
         <v>46018</v>
       </c>
-      <c r="I108" s="108"/>
-      <c r="J108" s="108"/>
-      <c r="K108" s="108"/>
-      <c r="L108" s="108">
+      <c r="L108" s="4">
         <v>-10000</v>
       </c>
-      <c r="M108" s="108"/>
+      <c r="M108" s="4"/>
       <c r="N108" s="92" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="2:14" ht="15">
+    <row r="109" spans="2:14" ht="14">
       <c r="B109" s="26">
         <v>46018</v>
       </c>
@@ -3205,19 +3120,17 @@
       <c r="H109" s="90">
         <v>46022</v>
       </c>
-      <c r="I109" s="108"/>
-      <c r="J109" s="108"/>
-      <c r="K109" s="108">
+      <c r="K109" s="4">
         <f>-3*184</f>
         <v>-552</v>
       </c>
-      <c r="L109" s="108"/>
-      <c r="M109" s="108"/>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
       <c r="N109" s="92" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="110" spans="2:14" ht="15">
+    <row r="110" spans="2:14" ht="14">
       <c r="B110" s="26">
         <v>46022</v>
       </c>
@@ -3231,19 +3144,17 @@
       <c r="H110" s="90">
         <v>46022</v>
       </c>
-      <c r="I110" s="108"/>
-      <c r="J110" s="108"/>
-      <c r="K110" s="108">
+      <c r="K110" s="4">
         <f>-3*CostBlocks25!$C$24</f>
         <v>-528</v>
       </c>
-      <c r="L110" s="108"/>
-      <c r="M110" s="108"/>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4"/>
       <c r="N110" s="92" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="111" spans="2:14" ht="15">
+    <row r="111" spans="2:14" ht="14">
       <c r="B111" s="26">
         <v>46022</v>
       </c>
@@ -3257,11 +3168,8 @@
       <c r="H111" s="90">
         <v>46022</v>
       </c>
-      <c r="I111" s="108"/>
-      <c r="J111" s="108"/>
-      <c r="K111" s="108"/>
-      <c r="L111" s="108"/>
-      <c r="M111" s="108">
+      <c r="L111" s="4"/>
+      <c r="M111" s="4">
         <f>-((J115+K115)*0.1)*1.02</f>
         <v>-6040.5420000000004</v>
       </c>
@@ -3269,7 +3177,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="112" spans="2:14" ht="15">
+    <row r="112" spans="2:14" ht="14">
       <c r="B112" s="26">
         <v>46022</v>
       </c>
@@ -3282,11 +3190,8 @@
       <c r="H112" s="90">
         <v>46022</v>
       </c>
-      <c r="I112" s="108"/>
-      <c r="J112" s="108"/>
-      <c r="K112" s="108"/>
-      <c r="L112" s="108"/>
-      <c r="M112" s="108">
+      <c r="L112" s="4"/>
+      <c r="M112" s="4">
         <f>(L115*0.05)*1.02-M48-M86</f>
         <v>-1601.7799999999997</v>
       </c>
@@ -3294,7 +3199,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="113" spans="2:14" ht="15">
+    <row r="113" spans="2:14" ht="14">
       <c r="B113" s="30">
         <v>46022</v>
       </c>
@@ -3318,13 +3223,13 @@
       <c r="M113" s="33"/>
       <c r="N113" s="34"/>
     </row>
-    <row r="114" spans="2:14" ht="15">
+    <row r="114" spans="2:14" ht="14">
       <c r="B114" s="5"/>
       <c r="C114" s="24"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
     </row>
-    <row r="115" spans="2:14" ht="15">
+    <row r="115" spans="2:14" ht="14">
       <c r="B115" s="35" t="s">
         <v>90</v>
       </c>
@@ -3355,236 +3260,236 @@
         <v>-14606.302</v>
       </c>
     </row>
-    <row r="116" spans="2:14" ht="15">
+    <row r="116" spans="2:14" ht="14">
       <c r="B116" s="38"/>
     </row>
-    <row r="117" spans="2:14" ht="15">
+    <row r="117" spans="2:14" ht="14">
       <c r="B117" s="38"/>
       <c r="G117" s="4"/>
     </row>
-    <row r="118" spans="2:14" ht="15">
+    <row r="118" spans="2:14" ht="14">
       <c r="B118" s="38"/>
     </row>
-    <row r="119" spans="2:14" ht="15">
+    <row r="119" spans="2:14" ht="14">
       <c r="B119" s="38"/>
     </row>
-    <row r="120" spans="2:14" ht="15">
+    <row r="120" spans="2:14" ht="14">
       <c r="B120" s="38"/>
       <c r="C120" s="24"/>
       <c r="F120" s="4"/>
     </row>
-    <row r="121" spans="2:14" ht="15">
+    <row r="121" spans="2:14" ht="14">
       <c r="B121" s="38"/>
     </row>
-    <row r="122" spans="2:14" ht="15">
+    <row r="122" spans="2:14" ht="14">
       <c r="B122" s="38"/>
       <c r="G122" s="4"/>
     </row>
-    <row r="123" spans="2:14" ht="15">
+    <row r="123" spans="2:14" ht="14">
       <c r="B123" s="38"/>
     </row>
-    <row r="124" spans="2:14" ht="15">
+    <row r="124" spans="2:14" ht="14">
       <c r="B124" s="38"/>
       <c r="G124" s="4"/>
     </row>
-    <row r="125" spans="2:14" ht="15">
+    <row r="125" spans="2:14" ht="14">
       <c r="B125" s="38"/>
     </row>
-    <row r="126" spans="2:14" ht="15">
+    <row r="126" spans="2:14" ht="14">
       <c r="B126" s="38"/>
     </row>
-    <row r="127" spans="2:14" ht="15">
+    <row r="127" spans="2:14" ht="14">
       <c r="B127" s="38"/>
       <c r="C127" s="24"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
     </row>
-    <row r="128" spans="2:14" ht="15">
+    <row r="128" spans="2:14" ht="14">
       <c r="B128" s="38"/>
       <c r="G128" s="4"/>
     </row>
-    <row r="129" spans="2:8" ht="15">
+    <row r="129" spans="2:8" ht="14">
       <c r="B129" s="38"/>
       <c r="F129" s="11"/>
     </row>
-    <row r="130" spans="2:8" ht="15">
+    <row r="130" spans="2:8" ht="14">
       <c r="B130" s="38"/>
     </row>
-    <row r="131" spans="2:8" ht="15">
+    <row r="131" spans="2:8" ht="14">
       <c r="B131" s="38"/>
     </row>
-    <row r="132" spans="2:8" ht="15">
+    <row r="132" spans="2:8" ht="14">
       <c r="B132" s="38"/>
       <c r="F132" s="4"/>
       <c r="G132" s="4"/>
     </row>
-    <row r="133" spans="2:8" ht="15">
+    <row r="133" spans="2:8" ht="14">
       <c r="B133" s="38"/>
       <c r="F133" s="11"/>
       <c r="G133" s="4"/>
     </row>
-    <row r="134" spans="2:8" ht="15">
+    <row r="134" spans="2:8" ht="14">
       <c r="B134" s="38"/>
       <c r="F134" s="11"/>
       <c r="G134" s="11"/>
     </row>
-    <row r="135" spans="2:8" ht="15">
+    <row r="135" spans="2:8" ht="14">
       <c r="G135" s="4"/>
     </row>
-    <row r="139" spans="2:8" ht="15">
-      <c r="B139" s="105"/>
-      <c r="C139" s="105"/>
-    </row>
-    <row r="140" spans="2:8" ht="15">
+    <row r="139" spans="2:8" ht="14">
+      <c r="B139" s="109"/>
+      <c r="C139" s="109"/>
+    </row>
+    <row r="140" spans="2:8" ht="14">
       <c r="F140" s="11"/>
       <c r="H140" s="39"/>
     </row>
-    <row r="141" spans="2:8" ht="15">
+    <row r="141" spans="2:8" ht="14">
       <c r="H141" s="39"/>
     </row>
-    <row r="142" spans="2:8" ht="15">
+    <row r="142" spans="2:8" ht="14">
       <c r="H142" s="39"/>
     </row>
-    <row r="143" spans="2:8" ht="15">
+    <row r="143" spans="2:8" ht="14">
       <c r="H143" s="39"/>
     </row>
-    <row r="144" spans="2:8" ht="15">
+    <row r="144" spans="2:8" ht="14">
       <c r="H144" s="39"/>
     </row>
-    <row r="145" spans="8:14" ht="15">
+    <row r="145" spans="8:14" ht="14">
       <c r="H145" s="39"/>
     </row>
-    <row r="146" spans="8:14" ht="15">
+    <row r="146" spans="8:14" ht="14">
       <c r="H146" s="39"/>
     </row>
-    <row r="147" spans="8:14" ht="15">
+    <row r="147" spans="8:14" ht="14">
       <c r="H147" s="39"/>
     </row>
-    <row r="148" spans="8:14" ht="15">
+    <row r="148" spans="8:14" ht="14">
       <c r="H148" s="39"/>
     </row>
-    <row r="149" spans="8:14" ht="15">
+    <row r="149" spans="8:14" ht="14">
       <c r="H149" s="39"/>
     </row>
-    <row r="150" spans="8:14" ht="15">
+    <row r="150" spans="8:14" ht="14">
       <c r="H150" s="39"/>
     </row>
-    <row r="151" spans="8:14" ht="15">
+    <row r="151" spans="8:14" ht="14">
       <c r="H151" s="39"/>
     </row>
-    <row r="153" spans="8:14" ht="15">
+    <row r="153" spans="8:14" ht="14">
       <c r="I153" s="38"/>
       <c r="J153" s="2"/>
       <c r="L153" s="40"/>
       <c r="M153" s="40"/>
     </row>
-    <row r="154" spans="8:14" ht="15">
+    <row r="154" spans="8:14" ht="14">
       <c r="I154" s="38"/>
       <c r="J154" s="2"/>
       <c r="L154" s="40"/>
       <c r="M154" s="40"/>
     </row>
-    <row r="155" spans="8:14" ht="15">
+    <row r="155" spans="8:14" ht="14">
       <c r="I155" s="38"/>
       <c r="J155" s="2"/>
       <c r="L155" s="40"/>
       <c r="M155" s="40"/>
     </row>
-    <row r="156" spans="8:14" ht="15">
+    <row r="156" spans="8:14" ht="14">
       <c r="I156" s="38"/>
       <c r="J156" s="2"/>
       <c r="L156" s="40"/>
       <c r="M156" s="40"/>
     </row>
-    <row r="157" spans="8:14" ht="15">
+    <row r="157" spans="8:14" ht="14">
       <c r="I157" s="38"/>
     </row>
-    <row r="158" spans="8:14" ht="15">
+    <row r="158" spans="8:14" ht="14">
       <c r="I158" s="38"/>
       <c r="N158" s="11"/>
     </row>
-    <row r="159" spans="8:14" ht="15">
+    <row r="159" spans="8:14" ht="14">
       <c r="I159" s="38"/>
       <c r="L159" s="40"/>
       <c r="M159" s="40"/>
       <c r="N159" s="11"/>
     </row>
-    <row r="160" spans="8:14" ht="15">
+    <row r="160" spans="8:14" ht="14">
       <c r="I160" s="38"/>
       <c r="L160" s="40"/>
       <c r="M160" s="40"/>
       <c r="N160" s="11"/>
     </row>
-    <row r="161" spans="3:14" ht="15">
+    <row r="161" spans="3:14" ht="14">
       <c r="I161" s="38"/>
       <c r="L161" s="40"/>
       <c r="M161" s="40"/>
       <c r="N161" s="11"/>
     </row>
-    <row r="162" spans="3:14" ht="15">
+    <row r="162" spans="3:14" ht="14">
       <c r="I162" s="38"/>
       <c r="N162" s="11"/>
     </row>
-    <row r="163" spans="3:14" ht="15">
+    <row r="163" spans="3:14" ht="14">
       <c r="I163" s="38"/>
       <c r="L163" s="40"/>
       <c r="M163" s="40"/>
       <c r="N163" s="11"/>
     </row>
-    <row r="164" spans="3:14" ht="15">
+    <row r="164" spans="3:14" ht="14">
       <c r="I164" s="38"/>
       <c r="N164" s="11"/>
     </row>
-    <row r="165" spans="3:14" ht="15">
+    <row r="165" spans="3:14" ht="14">
       <c r="I165" s="38"/>
       <c r="L165" s="40"/>
       <c r="M165" s="40"/>
       <c r="N165" s="11"/>
     </row>
-    <row r="166" spans="3:14" ht="15">
+    <row r="166" spans="3:14" ht="14">
       <c r="I166" s="38"/>
       <c r="L166" s="40"/>
       <c r="M166" s="40"/>
       <c r="N166" s="11"/>
     </row>
-    <row r="167" spans="3:14" ht="15">
+    <row r="167" spans="3:14" ht="14">
       <c r="I167" s="38"/>
       <c r="L167" s="40"/>
       <c r="M167" s="40"/>
       <c r="N167" s="11"/>
     </row>
-    <row r="168" spans="3:14" ht="15">
+    <row r="168" spans="3:14" ht="14">
       <c r="I168" s="38"/>
     </row>
-    <row r="169" spans="3:14" ht="15">
+    <row r="169" spans="3:14" ht="14">
       <c r="I169" s="38"/>
     </row>
-    <row r="170" spans="3:14" ht="15">
+    <row r="170" spans="3:14" ht="14">
       <c r="I170" s="38"/>
     </row>
-    <row r="171" spans="3:14" ht="15">
+    <row r="171" spans="3:14" ht="14">
       <c r="I171" s="41"/>
     </row>
-    <row r="172" spans="3:14" ht="15">
+    <row r="172" spans="3:14" ht="14">
       <c r="F172" s="11"/>
       <c r="I172" s="38"/>
       <c r="N172" s="11"/>
     </row>
-    <row r="173" spans="3:14" ht="15">
+    <row r="173" spans="3:14" ht="14">
       <c r="C173" s="37"/>
       <c r="D173" s="37"/>
       <c r="F173" s="11"/>
       <c r="I173" s="38"/>
     </row>
-    <row r="174" spans="3:14" ht="15">
+    <row r="174" spans="3:14" ht="14">
       <c r="I174" s="38"/>
       <c r="N174" s="11"/>
     </row>
-    <row r="175" spans="3:14" ht="15">
+    <row r="175" spans="3:14" ht="14">
       <c r="I175" s="38"/>
       <c r="N175" s="11"/>
     </row>
-    <row r="176" spans="3:14" ht="15">
+    <row r="176" spans="3:14" ht="14">
       <c r="I176" s="38"/>
       <c r="N176" s="11"/>
     </row>
@@ -3610,7 +3515,7 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.1640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
@@ -3635,26 +3540,26 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="6" customHeight="1"/>
-    <row r="4" spans="2:15" ht="16">
+    <row r="4" spans="2:15" ht="15">
       <c r="B4" s="44" t="s">
         <v>92</v>
       </c>
       <c r="E4" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="106" t="s">
+      <c r="H4" s="110" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="106"/>
-      <c r="K4" s="106" t="s">
+      <c r="I4" s="110"/>
+      <c r="K4" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="L4" s="106"/>
+      <c r="L4" s="110"/>
       <c r="M4" s="45"/>
-      <c r="N4" s="106" t="s">
+      <c r="N4" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="106"/>
+      <c r="O4" s="110"/>
     </row>
     <row r="5" spans="2:15" ht="6" customHeight="1">
       <c r="B5" s="46"/>

</xml_diff>

<commit_message>
bank statements DSK for August 2025
small planning adjustments
</commit_message>
<xml_diff>
--- a/Planning/overview_planning_25.xlsx
+++ b/Planning/overview_planning_25.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernd/financials/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BA798C-0A21-F24C-AE14-EE1E85792EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993B6332-0985-1D45-AD6A-2950D3951300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:AMC174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.5" customHeight="1"/>
@@ -2945,7 +2945,7 @@
         <v>45930</v>
       </c>
       <c r="D100" s="4">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="F100" s="92" t="s">
         <v>158</v>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="C103" s="18">
         <f>SUM(C96:E102)</f>
-        <v>38580.200000000004</v>
+        <v>38655.200000000004</v>
       </c>
       <c r="D103" s="18"/>
       <c r="E103" s="18"/>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="C111" s="31">
         <f>SUM(C103:E110)</f>
-        <v>58828.700000000004</v>
+        <v>58903.700000000004</v>
       </c>
       <c r="D111" s="31"/>
       <c r="E111" s="31"/>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="C113" s="36">
         <f>C111+P111+I111</f>
-        <v>59571.228000000003</v>
+        <v>59646.228000000003</v>
       </c>
       <c r="D113" s="36"/>
       <c r="E113" s="36"/>

</xml_diff>

<commit_message>
overview planning -> moved Da Nang to Q1 2026, add Bengaluru in Q4 2025 (Nov-Dec)
</commit_message>
<xml_diff>
--- a/Planning/overview_planning_25.xlsx
+++ b/Planning/overview_planning_25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernd/financials/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B3212B-C6CD-1F4A-B03A-8895D39A7BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76ADFCFA-846A-1E43-AC82-DAFF4A8C1AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="30120" windowHeight="33220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="34200" windowHeight="21440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview25" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
   <si>
     <t>Financial overview plan 2025</t>
   </si>
@@ -291,12 +291,6 @@
     <t>Monthly costs Q3</t>
   </si>
   <si>
-    <t>SustSol 25p5</t>
-  </si>
-  <si>
-    <t>AI Inference (Hetz)</t>
-  </si>
-  <si>
     <t>Monthly costs Q4</t>
   </si>
   <si>
@@ -327,9 +321,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Umsatz 2024</t>
-  </si>
-  <si>
     <t>Thailand (9.1. - 7.2.)</t>
   </si>
   <si>
@@ -342,9 +333,6 @@
     <t>Kitchen Castle</t>
   </si>
   <si>
-    <t>SustSol Q1</t>
-  </si>
-  <si>
     <t>Flight</t>
   </si>
   <si>
@@ -357,9 +345,6 @@
     <t>Castlen</t>
   </si>
   <si>
-    <t>SustSol Q2</t>
-  </si>
-  <si>
     <t>Airbnb</t>
   </si>
   <si>
@@ -369,21 +354,12 @@
     <t>Ohr-Bite</t>
   </si>
   <si>
-    <t>SustSol Q3</t>
-  </si>
-  <si>
     <t>Life</t>
   </si>
   <si>
     <t>Airports</t>
   </si>
   <si>
-    <t>Micro-backroar</t>
-  </si>
-  <si>
-    <t>SustSol Q4</t>
-  </si>
-  <si>
     <t>Transportation (Airport Van)</t>
   </si>
   <si>
@@ -432,9 +408,6 @@
     <t>Langkawi Trip (22.-29.4.)</t>
   </si>
   <si>
-    <t>BG Company montly expenses</t>
-  </si>
-  <si>
     <t>2025 Q1 Travel Expenses</t>
   </si>
   <si>
@@ -522,12 +495,6 @@
     <t>Lisi Credit</t>
   </si>
   <si>
-    <t>Da Nang (Nov. - Jan.)</t>
-  </si>
-  <si>
-    <t>Thailand (few days)</t>
-  </si>
-  <si>
     <t>Da Nang (2M in 2025)</t>
   </si>
   <si>
@@ -535,6 +502,48 @@
   </si>
   <si>
     <t>Mac Mini</t>
+  </si>
+  <si>
+    <t>Tiger Revenue</t>
+  </si>
+  <si>
+    <t>Reading Glasses</t>
+  </si>
+  <si>
+    <t>SG Incorporation</t>
+  </si>
+  <si>
+    <t>Da Nang (Jan. - Mar.)</t>
+  </si>
+  <si>
+    <t>CostBlocks 2026</t>
+  </si>
+  <si>
+    <t>Apt. + Cow.</t>
+  </si>
+  <si>
+    <t>Mike-backroar</t>
+  </si>
+  <si>
+    <t>Totel</t>
+  </si>
+  <si>
+    <t>Trips (4x)</t>
+  </si>
+  <si>
+    <t>Bangkok (few days)</t>
+  </si>
+  <si>
+    <t>Hue Rail+Hotel+Boat+Grab</t>
+  </si>
+  <si>
+    <t>Hetzner + Hosting + AI</t>
+  </si>
+  <si>
+    <t>Bangalore (Nov-Dec)</t>
+  </si>
+  <si>
+    <t>BG Company monthly expenses</t>
   </si>
 </sst>
 </file>
@@ -550,7 +559,7 @@
     <numFmt numFmtId="169" formatCode="[$€-C07]\ #,##0.00"/>
     <numFmt numFmtId="170" formatCode="[$EUR]\ #,##0.00;[Red][$EUR]\ #,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,6 +688,19 @@
       <color theme="1"/>
       <name val="Liberation Sans11"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="LiterationSerif Nerd Font"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="LiterationSerif Nerd Font"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="22">
     <fill>
@@ -724,12 +746,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor rgb="FF404040"/>
       </patternFill>
@@ -738,12 +754,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00662C"/>
         <bgColor indexed="21"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59978026673177287"/>
-        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -762,12 +772,6 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="0.39979247413556324"/>
         <bgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="52"/>
       </patternFill>
     </fill>
     <fill>
@@ -804,6 +808,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC8102E"/>
         <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9933"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -945,7 +967,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1022,46 +1044,33 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="18" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="18" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="10" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="14" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="14" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="14" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="10" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="20" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="10" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="10" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="14" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="14" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="19" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="10" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="14" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="10" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="14" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="10" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="14" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="14" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="17" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="10" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="20" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="10" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="10" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="14" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="14" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="19" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="14" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="10" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="14" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="10" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="14" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="20" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1072,14 +1081,14 @@
     <xf numFmtId="168" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="18" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="18" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="18" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="18" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="18" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="18" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="17" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="10" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -1093,6 +1102,20 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="10" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="14" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="23" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="22" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="10" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="13" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="14" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent 1 5" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -1114,6 +1137,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9933"/>
       <color rgb="FF2D2A4A"/>
       <color rgb="FFC8102E"/>
       <color rgb="FFDA251D"/>
@@ -1301,10 +1325,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMC173"/>
+  <dimension ref="A1:AMC175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13.5" customHeight="1"/>
@@ -1312,8 +1336,9 @@
     <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="5" customWidth="1"/>
     <col min="9" max="9" width="10" style="4" bestFit="1" customWidth="1"/>
@@ -1328,12 +1353,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="20">
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
     </row>
     <row r="3" spans="2:14" ht="15">
       <c r="B3" s="7" t="s">
@@ -1373,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>6</v>
@@ -1382,7 +1407,7 @@
         <v>8</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="N5" s="14" t="s">
         <v>7</v>
@@ -1921,7 +1946,7 @@
         <v>45747</v>
       </c>
       <c r="K39" s="4">
-        <f>-3*CostBlocks25!$C$24</f>
+        <f>-3*CostBlocks25!$C$17</f>
         <v>-528</v>
       </c>
       <c r="L39" s="4"/>
@@ -2091,7 +2116,7 @@
         <v>-436.86</v>
       </c>
       <c r="N48" s="27" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="15">
@@ -2115,7 +2140,7 @@
         <v>45779</v>
       </c>
       <c r="E50" s="4">
-        <f>-CostBlocks25!$C$19</f>
+        <f>-CostBlocks25!$C$12</f>
         <v>-605</v>
       </c>
       <c r="F50" s="28" t="s">
@@ -2262,8 +2287,8 @@
       <c r="F60" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H60" s="89"/>
-      <c r="N60" s="92"/>
+      <c r="H60" s="76"/>
+      <c r="N60" s="79"/>
     </row>
     <row r="61" spans="2:14" ht="15">
       <c r="B61" s="26">
@@ -2275,8 +2300,8 @@
       <c r="F61" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H61" s="89"/>
-      <c r="N61" s="92"/>
+      <c r="H61" s="76"/>
+      <c r="N61" s="79"/>
     </row>
     <row r="62" spans="2:14" ht="15">
       <c r="B62" s="26">
@@ -2288,10 +2313,10 @@
       <c r="F62" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H62" s="90"/>
+      <c r="H62" s="77"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
-      <c r="N62" s="93"/>
+      <c r="N62" s="80"/>
     </row>
     <row r="63" spans="2:14" ht="15">
       <c r="B63" s="20">
@@ -2304,10 +2329,10 @@
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="22"/>
-      <c r="H63" s="90"/>
+      <c r="H63" s="77"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
-      <c r="N63" s="92"/>
+      <c r="N63" s="79"/>
     </row>
     <row r="64" spans="2:14" ht="15">
       <c r="B64" s="26">
@@ -2319,8 +2344,8 @@
       <c r="F64" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H64" s="89"/>
-      <c r="N64" s="92"/>
+      <c r="H64" s="76"/>
+      <c r="N64" s="79"/>
     </row>
     <row r="65" spans="2:14" ht="15">
       <c r="B65" s="26">
@@ -2332,10 +2357,10 @@
       <c r="F65" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="H65" s="90"/>
+      <c r="H65" s="77"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
-      <c r="N65" s="93"/>
+      <c r="N65" s="80"/>
     </row>
     <row r="66" spans="2:14" ht="15">
       <c r="B66" s="26">
@@ -2347,7 +2372,7 @@
       <c r="F66" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="90">
+      <c r="H66" s="77">
         <v>45812</v>
       </c>
       <c r="J66" s="4">
@@ -2355,7 +2380,7 @@
       </c>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="N66" s="93" t="s">
+      <c r="N66" s="80" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2372,14 +2397,14 @@
       <c r="F67" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="H67" s="90">
+      <c r="H67" s="77">
         <v>45812</v>
       </c>
       <c r="L67" s="4">
         <v>-10200</v>
       </c>
       <c r="M67" s="4"/>
-      <c r="N67" s="92" t="s">
+      <c r="N67" s="79" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2393,10 +2418,10 @@
       <c r="F68" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="H68" s="90"/>
+      <c r="H68" s="77"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
-      <c r="N68" s="93"/>
+      <c r="N68" s="80"/>
     </row>
     <row r="69" spans="2:14" ht="15">
       <c r="B69" s="26">
@@ -2408,10 +2433,10 @@
       <c r="F69" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H69" s="90"/>
+      <c r="H69" s="77"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
-      <c r="N69" s="93"/>
+      <c r="N69" s="80"/>
     </row>
     <row r="70" spans="2:14" ht="15">
       <c r="B70" s="20">
@@ -2424,10 +2449,10 @@
       <c r="D70" s="18"/>
       <c r="E70" s="18"/>
       <c r="F70" s="22"/>
-      <c r="H70" s="90"/>
+      <c r="H70" s="77"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
-      <c r="N70" s="93"/>
+      <c r="N70" s="80"/>
     </row>
     <row r="71" spans="2:14" ht="15">
       <c r="B71" s="26">
@@ -2439,10 +2464,10 @@
       <c r="F71" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="H71" s="90"/>
+      <c r="H71" s="77"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
-      <c r="N71" s="93"/>
+      <c r="N71" s="80"/>
     </row>
     <row r="72" spans="2:14" ht="15">
       <c r="B72" s="26">
@@ -2454,13 +2479,13 @@
       <c r="F72" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H72" s="91"/>
+      <c r="H72" s="78"/>
       <c r="I72"/>
       <c r="J72"/>
       <c r="K72"/>
       <c r="L72"/>
       <c r="M72"/>
-      <c r="N72" s="94"/>
+      <c r="N72" s="81"/>
     </row>
     <row r="73" spans="2:14" ht="15">
       <c r="B73" s="26">
@@ -2472,13 +2497,13 @@
       <c r="F73" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="H73" s="91"/>
+      <c r="H73" s="78"/>
       <c r="I73"/>
       <c r="J73"/>
       <c r="K73"/>
       <c r="L73"/>
       <c r="M73"/>
-      <c r="N73" s="94"/>
+      <c r="N73" s="81"/>
     </row>
     <row r="74" spans="2:14" ht="15">
       <c r="B74" s="26">
@@ -2490,14 +2515,14 @@
       <c r="F74" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="H74" s="90">
+      <c r="H74" s="77">
         <v>45838</v>
       </c>
       <c r="L74" s="4"/>
       <c r="M74" s="4">
         <v>-4707.47</v>
       </c>
-      <c r="N74" s="92" t="s">
+      <c r="N74" s="79" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2506,22 +2531,22 @@
         <v>45838</v>
       </c>
       <c r="E75" s="4">
-        <f>-3*CostBlocks25!$C$19+E61-E69-52</f>
+        <f>-3*CostBlocks25!$C$12+E61-E69-52</f>
         <v>-617</v>
       </c>
       <c r="F75" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="H75" s="90">
+      <c r="H75" s="77">
         <v>45838</v>
       </c>
       <c r="K75" s="4">
-        <f>-3*CostBlocks25!$C$24</f>
+        <f>-3*CostBlocks25!$C$17</f>
         <v>-528</v>
       </c>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
-      <c r="N75" s="92" t="s">
+      <c r="N75" s="79" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2535,8 +2560,8 @@
       <c r="F76" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="H76" s="89"/>
-      <c r="N76" s="92"/>
+      <c r="H76" s="76"/>
+      <c r="N76" s="79"/>
     </row>
     <row r="77" spans="2:14" ht="15">
       <c r="B77" s="26">
@@ -2548,8 +2573,8 @@
       <c r="F77" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="H77" s="89"/>
-      <c r="N77" s="92"/>
+      <c r="H77" s="76"/>
+      <c r="N77" s="79"/>
     </row>
     <row r="78" spans="2:14" ht="15">
       <c r="B78" s="26">
@@ -2561,10 +2586,10 @@
       <c r="F78" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="H78" s="90"/>
+      <c r="H78" s="77"/>
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
-      <c r="N78" s="93"/>
+      <c r="N78" s="80"/>
     </row>
     <row r="79" spans="2:14" ht="15">
       <c r="B79" s="26">
@@ -2577,10 +2602,10 @@
       <c r="F79" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="H79" s="90"/>
+      <c r="H79" s="77"/>
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
-      <c r="N79" s="93"/>
+      <c r="N79" s="80"/>
     </row>
     <row r="80" spans="2:14" ht="15">
       <c r="B80" s="26">
@@ -2600,8 +2625,8 @@
       </c>
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
-      <c r="N80" s="93" t="s">
-        <v>145</v>
+      <c r="N80" s="80" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="2:14" ht="15">
@@ -2621,7 +2646,7 @@
         <v>171.21</v>
       </c>
       <c r="N81" s="28" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="82" spans="2:14" ht="15">
@@ -2632,7 +2657,7 @@
         <v>-428</v>
       </c>
       <c r="F82" s="27" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="H82" s="26">
         <v>45854</v>
@@ -2641,7 +2666,7 @@
         <v>428</v>
       </c>
       <c r="N82" s="28" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="2:14" ht="15">
@@ -2676,7 +2701,7 @@
         <v>-275</v>
       </c>
       <c r="F84" s="27" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="H84" s="26"/>
       <c r="L84" s="11"/>
@@ -2691,7 +2716,7 @@
         <v>-300</v>
       </c>
       <c r="F85" s="27" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="H85" s="26"/>
       <c r="L85" s="11"/>
@@ -2706,7 +2731,7 @@
         <v>-300</v>
       </c>
       <c r="F86" s="27" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="H86" s="26">
         <v>45866</v>
@@ -2716,7 +2741,7 @@
         <v>-536.86</v>
       </c>
       <c r="N86" s="27" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="2:14" ht="15">
@@ -2727,7 +2752,7 @@
         <v>-3016.58</v>
       </c>
       <c r="F87" s="28" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H87" s="26">
         <v>45869</v>
@@ -2738,7 +2763,7 @@
       <c r="L87" s="11"/>
       <c r="M87" s="4"/>
       <c r="N87" s="27" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="2:14" ht="15">
@@ -2751,10 +2776,10 @@
       <c r="F88" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="H88" s="90"/>
+      <c r="H88" s="77"/>
       <c r="L88" s="11"/>
       <c r="M88" s="4"/>
-      <c r="N88" s="93"/>
+      <c r="N88" s="80"/>
     </row>
     <row r="89" spans="2:14" ht="15">
       <c r="B89" s="26">
@@ -2764,12 +2789,12 @@
         <v>-120</v>
       </c>
       <c r="F89" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="H89" s="90"/>
+        <v>147</v>
+      </c>
+      <c r="H89" s="77"/>
       <c r="L89" s="11"/>
       <c r="M89" s="4"/>
-      <c r="N89" s="93"/>
+      <c r="N89" s="80"/>
     </row>
     <row r="90" spans="2:14" ht="15">
       <c r="B90" s="26">
@@ -2779,12 +2804,12 @@
         <v>-100</v>
       </c>
       <c r="F90" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="H90" s="90"/>
+        <v>148</v>
+      </c>
+      <c r="H90" s="77"/>
       <c r="L90" s="11"/>
       <c r="M90" s="4"/>
-      <c r="N90" s="93"/>
+      <c r="N90" s="80"/>
     </row>
     <row r="91" spans="2:14" ht="15">
       <c r="B91" s="20">
@@ -2797,8 +2822,8 @@
       <c r="D91" s="18"/>
       <c r="E91" s="18"/>
       <c r="F91" s="22"/>
-      <c r="H91" s="89"/>
-      <c r="N91" s="92"/>
+      <c r="H91" s="76"/>
+      <c r="N91" s="79"/>
     </row>
     <row r="92" spans="2:14" ht="15">
       <c r="B92" s="26">
@@ -2807,11 +2832,11 @@
       <c r="E92" s="4">
         <v>-882</v>
       </c>
-      <c r="F92" s="93" t="s">
-        <v>159</v>
-      </c>
-      <c r="H92" s="89"/>
-      <c r="N92" s="92"/>
+      <c r="F92" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="H92" s="76"/>
+      <c r="N92" s="79"/>
     </row>
     <row r="93" spans="2:14" ht="15">
       <c r="B93" s="26">
@@ -2820,36 +2845,26 @@
       <c r="E93" s="4">
         <v>-243</v>
       </c>
-      <c r="F93" s="93" t="s">
-        <v>160</v>
-      </c>
-      <c r="H93" s="89"/>
-      <c r="I93" s="111"/>
-      <c r="J93" s="111"/>
-      <c r="K93" s="111"/>
-      <c r="L93" s="112"/>
-      <c r="M93" s="112"/>
-      <c r="N93" s="92"/>
+      <c r="F93" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="H93" s="76"/>
+      <c r="N93" s="79"/>
     </row>
     <row r="94" spans="2:14" ht="15">
       <c r="B94" s="26">
         <v>45894</v>
       </c>
       <c r="C94" s="1"/>
-      <c r="D94" s="106"/>
+      <c r="D94" s="93"/>
       <c r="E94" s="4">
         <v>-2000</v>
       </c>
-      <c r="F94" s="93" t="s">
-        <v>161</v>
-      </c>
-      <c r="H94" s="89"/>
-      <c r="I94" s="111"/>
-      <c r="J94" s="111"/>
-      <c r="K94" s="111"/>
-      <c r="L94" s="112"/>
-      <c r="M94" s="112"/>
-      <c r="N94" s="92"/>
+      <c r="F94" s="80" t="s">
+        <v>152</v>
+      </c>
+      <c r="H94" s="76"/>
+      <c r="N94" s="79"/>
     </row>
     <row r="95" spans="2:14" ht="15">
       <c r="B95" s="26">
@@ -2858,451 +2873,464 @@
       <c r="E95" s="4">
         <v>-360</v>
       </c>
-      <c r="F95" s="93" t="s">
-        <v>165</v>
-      </c>
-      <c r="H95" s="89"/>
-      <c r="I95" s="111"/>
-      <c r="J95" s="111"/>
-      <c r="K95" s="111"/>
-      <c r="L95" s="112"/>
-      <c r="M95" s="112"/>
-      <c r="N95" s="92"/>
+      <c r="F95" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="H95" s="76"/>
+      <c r="N95" s="79"/>
     </row>
     <row r="96" spans="2:14" ht="15">
       <c r="B96" s="26">
-        <v>45900</v>
+        <v>45904</v>
       </c>
       <c r="E96" s="4">
-        <v>-900</v>
+        <v>-1000</v>
       </c>
       <c r="F96" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="H96" s="89"/>
-      <c r="I96" s="111"/>
-      <c r="J96" s="111"/>
-      <c r="K96" s="111"/>
-      <c r="L96" s="112"/>
-      <c r="M96" s="112"/>
-      <c r="N96" s="92"/>
+      <c r="H96" s="76"/>
+      <c r="N96" s="79"/>
     </row>
     <row r="97" spans="2:14" ht="15">
-      <c r="B97" s="20">
-        <v>45902</v>
-      </c>
-      <c r="C97" s="18">
-        <f>SUM(C91:E96)</f>
-        <v>29450.520000000004</v>
-      </c>
-      <c r="D97" s="18"/>
-      <c r="E97" s="18"/>
-      <c r="F97" s="107"/>
-      <c r="H97" s="90">
-        <v>45902</v>
-      </c>
-      <c r="I97" s="111"/>
-      <c r="J97" s="111">
+      <c r="B97" s="26">
+        <v>45904</v>
+      </c>
+      <c r="E97" s="4">
+        <f>-42-20-28-20</f>
+        <v>-110</v>
+      </c>
+      <c r="F97" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="H97" s="76"/>
+      <c r="N97" s="79"/>
+    </row>
+    <row r="98" spans="2:14" ht="15">
+      <c r="B98" s="20">
+        <v>45904</v>
+      </c>
+      <c r="C98" s="18">
+        <f>SUM(C91:E97)</f>
+        <v>29240.520000000004</v>
+      </c>
+      <c r="D98" s="18"/>
+      <c r="E98" s="18"/>
+      <c r="F98" s="94"/>
+      <c r="H98" s="77">
+        <v>45904</v>
+      </c>
+      <c r="J98" s="4">
         <v>18000</v>
       </c>
-      <c r="K97" s="111"/>
-      <c r="L97" s="111"/>
-      <c r="M97" s="111"/>
-      <c r="N97" s="92" t="s">
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="79" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="98" spans="2:14" ht="15">
-      <c r="B98" s="26">
-        <v>45905</v>
-      </c>
-      <c r="D98" s="4">
-        <v>13000</v>
-      </c>
-      <c r="F98" s="92" t="s">
-        <v>8</v>
-      </c>
-      <c r="H98" s="90">
-        <v>45904</v>
-      </c>
-      <c r="I98" s="111"/>
-      <c r="J98" s="111"/>
-      <c r="K98" s="111"/>
-      <c r="L98" s="111">
-        <v>-13000</v>
-      </c>
-      <c r="M98" s="111"/>
-      <c r="N98" s="92" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="99" spans="2:14" ht="15">
       <c r="B99" s="26">
-        <v>45930</v>
+        <v>45905</v>
       </c>
       <c r="D99" s="4">
-        <v>225</v>
-      </c>
-      <c r="F99" s="92" t="s">
-        <v>158</v>
-      </c>
-      <c r="H99" s="90"/>
-      <c r="L99" s="4"/>
+        <v>15000</v>
+      </c>
+      <c r="F99" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="H99" s="77">
+        <v>45904</v>
+      </c>
+      <c r="L99" s="4">
+        <v>-15000</v>
+      </c>
       <c r="M99" s="4"/>
-      <c r="N99" s="92"/>
+      <c r="N99" s="79" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="100" spans="2:14" ht="15">
       <c r="B100" s="26">
-        <v>45930</v>
+        <v>45905</v>
       </c>
       <c r="E100" s="4">
-        <f>-CostBlocks25!$L$15-E67-E80/2-E81-E77-E85-E79-E84-E86-E88/2-E96/2</f>
-        <v>-1545.3200000000002</v>
-      </c>
-      <c r="F100" s="92" t="s">
-        <v>151</v>
-      </c>
-      <c r="H100" s="90"/>
-      <c r="N100" s="92"/>
+        <v>-250</v>
+      </c>
+      <c r="F100" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="H100" s="76"/>
+      <c r="I100" s="98"/>
+      <c r="J100" s="98"/>
+      <c r="K100" s="98"/>
+      <c r="L100" s="99"/>
+      <c r="M100" s="99"/>
+      <c r="N100" s="79"/>
     </row>
     <row r="101" spans="2:14" ht="15">
       <c r="B101" s="26">
         <v>45930</v>
       </c>
-      <c r="E101" s="4">
-        <f>-3*CostBlocks25!$C$19-E80/2-E88/2-E96/2</f>
-        <v>-715</v>
-      </c>
-      <c r="F101" s="92" t="s">
-        <v>84</v>
-      </c>
-      <c r="H101" s="90">
-        <v>45930</v>
-      </c>
-      <c r="K101" s="4">
-        <f>-3*CostBlocks25!$C$24-K80</f>
-        <v>-371</v>
-      </c>
+      <c r="D101" s="4">
+        <v>225</v>
+      </c>
+      <c r="F101" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="H101" s="77"/>
       <c r="L101" s="4"/>
       <c r="M101" s="4"/>
-      <c r="N101" s="92" t="s">
-        <v>45</v>
-      </c>
+      <c r="N101" s="79"/>
     </row>
     <row r="102" spans="2:14" ht="15">
-      <c r="B102" s="20">
-        <v>45931</v>
-      </c>
-      <c r="C102" s="18">
-        <f>SUM(C97:E101)</f>
-        <v>40415.200000000004</v>
-      </c>
-      <c r="D102" s="18"/>
-      <c r="E102" s="18"/>
-      <c r="F102" s="22"/>
-      <c r="H102" s="105">
-        <v>45962</v>
-      </c>
-      <c r="I102" s="18">
-        <f>SUM(I83:M101)</f>
-        <v>4864.8499999999985</v>
-      </c>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="29"/>
-      <c r="M102" s="29"/>
-      <c r="N102" s="104"/>
+      <c r="B102" s="26">
+        <v>45930</v>
+      </c>
+      <c r="E102" s="4">
+        <f>-CostBlocks25!$L$15-E67-E80/2-E81-E77-E85-E79-E84-E86-E88/2-E96/2-E97</f>
+        <v>-890.32000000000016</v>
+      </c>
+      <c r="F102" s="79" t="s">
+        <v>142</v>
+      </c>
+      <c r="H102" s="77"/>
+      <c r="N102" s="79"/>
     </row>
     <row r="103" spans="2:14" ht="15">
       <c r="B103" s="26">
-        <v>45938</v>
-      </c>
-      <c r="D103" s="4">
-        <v>1650</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="H103" s="89"/>
-      <c r="N103" s="92"/>
+        <v>45930</v>
+      </c>
+      <c r="E103" s="4">
+        <f>-3*CostBlocks25!$C$12-E80/2-E88/2-E96/2</f>
+        <v>-665</v>
+      </c>
+      <c r="F103" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="H103" s="77">
+        <v>45930</v>
+      </c>
+      <c r="K103" s="4">
+        <f>-3*CostBlocks25!$C$17-K80</f>
+        <v>-371</v>
+      </c>
+      <c r="L103" s="4"/>
+      <c r="M103" s="4"/>
+      <c r="N103" s="79" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="104" spans="2:14" ht="15">
-      <c r="B104" s="26"/>
-      <c r="F104" s="28"/>
-      <c r="H104" s="90">
-        <v>46011</v>
-      </c>
-      <c r="J104" s="4">
-        <v>18000</v>
-      </c>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="93" t="s">
-        <v>85</v>
-      </c>
+      <c r="B104" s="20">
+        <v>45931</v>
+      </c>
+      <c r="C104" s="18">
+        <f>SUM(C98:E103)</f>
+        <v>42660.200000000004</v>
+      </c>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="22"/>
+      <c r="H104" s="92">
+        <v>45962</v>
+      </c>
+      <c r="I104" s="18">
+        <f>SUM(I83:M103)</f>
+        <v>2864.8499999999985</v>
+      </c>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="29"/>
+      <c r="M104" s="29"/>
+      <c r="N104" s="91"/>
     </row>
     <row r="105" spans="2:14" ht="15">
       <c r="B105" s="26">
-        <v>45960</v>
-      </c>
-      <c r="E105" s="4">
-        <v>-500</v>
-      </c>
-      <c r="F105" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="H105" s="90">
-        <v>46018</v>
-      </c>
-      <c r="L105" s="4">
-        <v>-14000</v>
-      </c>
-      <c r="M105" s="4"/>
-      <c r="N105" s="92" t="s">
-        <v>8</v>
-      </c>
+        <v>45938</v>
+      </c>
+      <c r="D105" s="4">
+        <v>1650</v>
+      </c>
+      <c r="F105" s="79" t="s">
+        <v>155</v>
+      </c>
+      <c r="H105" s="76"/>
+      <c r="N105" s="79"/>
     </row>
     <row r="106" spans="2:14" ht="15">
       <c r="B106" s="26">
-        <v>45966</v>
+        <v>45938</v>
       </c>
       <c r="E106" s="4">
-        <v>-606.5</v>
+        <v>-3000</v>
       </c>
       <c r="F106" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="H106" s="90">
-        <v>46022</v>
-      </c>
-      <c r="K106" s="4">
-        <f>-3*184</f>
-        <v>-552</v>
-      </c>
-      <c r="L106" s="4"/>
-      <c r="M106" s="4"/>
-      <c r="N106" s="92" t="s">
-        <v>86</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="H106" s="76"/>
+      <c r="I106" s="98"/>
+      <c r="J106" s="98"/>
+      <c r="K106" s="98"/>
+      <c r="L106" s="99"/>
+      <c r="M106" s="99"/>
+      <c r="N106" s="79"/>
     </row>
     <row r="107" spans="2:14" ht="15">
       <c r="B107" s="26">
-        <v>46018</v>
-      </c>
-      <c r="D107" s="4">
-        <v>14000</v>
+        <v>45960</v>
+      </c>
+      <c r="E107" s="4">
+        <v>-500</v>
       </c>
       <c r="F107" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="H107" s="90">
-        <v>46022</v>
-      </c>
-      <c r="K107" s="4">
-        <f>-3*CostBlocks25!$C$24</f>
-        <v>-528</v>
+        <v>165</v>
+      </c>
+      <c r="H107" s="77">
+        <v>46011</v>
+      </c>
+      <c r="J107" s="4">
+        <v>10000</v>
       </c>
       <c r="L107" s="4"/>
       <c r="M107" s="4"/>
-      <c r="N107" s="92" t="s">
-        <v>45</v>
+      <c r="N107" s="80" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="108" spans="2:14" ht="15">
       <c r="B108" s="26">
-        <v>46022</v>
+        <v>45966</v>
       </c>
       <c r="E108" s="4">
-        <f>-CostBlocks25!$L$24*2/3</f>
-        <v>-1830</v>
+        <v>-606.5</v>
       </c>
       <c r="F108" s="28" t="s">
-        <v>164</v>
-      </c>
-      <c r="H108" s="90">
-        <v>46022</v>
-      </c>
-      <c r="L108" s="4"/>
-      <c r="M108" s="4">
-        <f>-((J112+K112)*0.1)*1.02</f>
-        <v>-5469.3420000000006</v>
-      </c>
-      <c r="N108" s="92" t="s">
-        <v>88</v>
+        <v>82</v>
+      </c>
+      <c r="H108" s="77">
+        <v>46018</v>
+      </c>
+      <c r="L108" s="4">
+        <v>-6000</v>
+      </c>
+      <c r="M108" s="4"/>
+      <c r="N108" s="79" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="2:14" ht="15">
       <c r="B109" s="26">
+        <v>46018</v>
+      </c>
+      <c r="D109" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F109" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H109" s="77">
         <v>46022</v>
       </c>
-      <c r="E109" s="4">
-        <f>-3*CostBlocks25!$C$19</f>
+      <c r="K109" s="4">
+        <f>-3*CostBlocks25!$C$17</f>
+        <v>-528</v>
+      </c>
+      <c r="L109" s="4"/>
+      <c r="M109" s="4"/>
+      <c r="N109" s="79" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="110" spans="2:14" ht="15">
+      <c r="B110" s="26">
+        <v>46022</v>
+      </c>
+      <c r="E110" s="4">
+        <f>-CostBlocks25!$L$24</f>
+        <v>-4680</v>
+      </c>
+      <c r="F110" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="H110" s="77">
+        <v>46022</v>
+      </c>
+      <c r="L110" s="4"/>
+      <c r="M110" s="4">
+        <f>-((J114+K114)*0.1)*1.02</f>
+        <v>-4709.6460000000006</v>
+      </c>
+      <c r="N110" s="79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="2:14" ht="15">
+      <c r="B111" s="26">
+        <v>46022</v>
+      </c>
+      <c r="E111" s="4">
+        <f>-3*CostBlocks25!$C$12</f>
         <v>-1815</v>
       </c>
-      <c r="F109" s="28" t="s">
+      <c r="F111" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="H111" s="77">
+        <v>46022</v>
+      </c>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4">
+        <f>(L114*0.05)*1.02-M48-M86</f>
+        <v>-1040.7799999999997</v>
+      </c>
+      <c r="N111" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="H109" s="90">
+    </row>
+    <row r="112" spans="2:14" ht="15">
+      <c r="B112" s="30">
         <v>46022</v>
       </c>
-      <c r="L109" s="4"/>
-      <c r="M109" s="4">
-        <f>(L112*0.05)*1.02-M48-M86</f>
-        <v>-1346.7799999999997</v>
-      </c>
-      <c r="N109" s="92" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" ht="15">
-      <c r="B110" s="30">
+      <c r="C112" s="31">
+        <f>SUM(C104:E111)</f>
+        <v>39708.700000000004</v>
+      </c>
+      <c r="D112" s="31"/>
+      <c r="E112" s="31"/>
+      <c r="F112" s="32"/>
+      <c r="H112" s="30">
         <v>46022</v>
       </c>
-      <c r="C110" s="31">
-        <f>SUM(C102:E109)</f>
-        <v>51313.700000000004</v>
-      </c>
-      <c r="D110" s="31"/>
-      <c r="E110" s="31"/>
-      <c r="F110" s="32"/>
-      <c r="H110" s="30">
-        <v>46022</v>
-      </c>
-      <c r="I110" s="31">
-        <f>SUM(I102:M109)</f>
-        <v>968.72799999999825</v>
-      </c>
-      <c r="J110" s="31"/>
-      <c r="K110" s="31"/>
-      <c r="L110" s="33"/>
-      <c r="M110" s="33"/>
-      <c r="N110" s="34"/>
-    </row>
-    <row r="111" spans="2:14" ht="15">
-      <c r="B111" s="5"/>
-      <c r="C111" s="24"/>
-      <c r="F111" s="4"/>
-      <c r="G111" s="4"/>
-    </row>
-    <row r="112" spans="2:14" ht="15">
-      <c r="B112" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C112" s="36">
-        <f>C110+P110+I110</f>
-        <v>52282.428</v>
-      </c>
-      <c r="D112" s="36"/>
-      <c r="E112" s="36"/>
-      <c r="G112" s="4"/>
-      <c r="I112" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="J112" s="37">
-        <f>SUM(J7:J109)</f>
-        <v>56800</v>
-      </c>
-      <c r="K112" s="37">
-        <f>SUM(K7:K109)</f>
-        <v>-3179</v>
-      </c>
-      <c r="L112" s="37">
-        <f t="shared" ref="L112:M112" si="0">SUM(L7:L109)</f>
-        <v>-45500</v>
-      </c>
-      <c r="M112" s="37">
+      <c r="I112" s="31">
+        <f>SUM(I104:M111)</f>
+        <v>586.42399999999816</v>
+      </c>
+      <c r="J112" s="31"/>
+      <c r="K112" s="31"/>
+      <c r="L112" s="33"/>
+      <c r="M112" s="33"/>
+      <c r="N112" s="34"/>
+    </row>
+    <row r="113" spans="2:13" ht="15">
+      <c r="B113" s="5"/>
+      <c r="C113" s="24"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+    </row>
+    <row r="114" spans="2:13" ht="15">
+      <c r="B114" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C114" s="36">
+        <f>C112+P112+I112</f>
+        <v>40295.124000000003</v>
+      </c>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
+      <c r="G114" s="4"/>
+      <c r="I114" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="J114" s="37">
+        <f>SUM(J7:J111)</f>
+        <v>48800</v>
+      </c>
+      <c r="K114" s="37">
+        <f>SUM(K7:K111)</f>
+        <v>-2627</v>
+      </c>
+      <c r="L114" s="37">
+        <f t="shared" ref="L114:M114" si="0">SUM(L7:L111)</f>
+        <v>-39500</v>
+      </c>
+      <c r="M114" s="37">
         <f t="shared" si="0"/>
-        <v>-13780.101999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" ht="15">
-      <c r="B113" s="38"/>
-    </row>
-    <row r="114" spans="2:7" ht="15">
-      <c r="B114" s="38"/>
-      <c r="G114" s="4"/>
-    </row>
-    <row r="115" spans="2:7" ht="15">
+        <v>-12714.405999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13" ht="15">
       <c r="B115" s="38"/>
     </row>
-    <row r="116" spans="2:7" ht="15">
+    <row r="116" spans="2:13" ht="15">
       <c r="B116" s="38"/>
-    </row>
-    <row r="117" spans="2:7" ht="15">
+      <c r="G116" s="4"/>
+    </row>
+    <row r="117" spans="2:13" ht="15">
       <c r="B117" s="38"/>
-      <c r="C117" s="24"/>
-      <c r="F117" s="4"/>
-    </row>
-    <row r="118" spans="2:7" ht="15">
+    </row>
+    <row r="118" spans="2:13" ht="15">
       <c r="B118" s="38"/>
     </row>
-    <row r="119" spans="2:7" ht="15">
+    <row r="119" spans="2:13" ht="15">
       <c r="B119" s="38"/>
-      <c r="G119" s="4"/>
-    </row>
-    <row r="120" spans="2:7" ht="15">
+      <c r="C119" s="24"/>
+      <c r="F119" s="4"/>
+    </row>
+    <row r="120" spans="2:13" ht="15">
       <c r="B120" s="38"/>
     </row>
-    <row r="121" spans="2:7" ht="15">
+    <row r="121" spans="2:13" ht="15">
       <c r="B121" s="38"/>
       <c r="G121" s="4"/>
     </row>
-    <row r="122" spans="2:7" ht="15">
+    <row r="122" spans="2:13" ht="15">
       <c r="B122" s="38"/>
     </row>
-    <row r="123" spans="2:7" ht="15">
+    <row r="123" spans="2:13" ht="15">
       <c r="B123" s="38"/>
-    </row>
-    <row r="124" spans="2:7" ht="15">
+      <c r="G123" s="4"/>
+    </row>
+    <row r="124" spans="2:13" ht="15">
       <c r="B124" s="38"/>
-      <c r="C124" s="24"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-    </row>
-    <row r="125" spans="2:7" ht="15">
+    </row>
+    <row r="125" spans="2:13" ht="15">
       <c r="B125" s="38"/>
-      <c r="G125" s="4"/>
-    </row>
-    <row r="126" spans="2:7" ht="15">
+    </row>
+    <row r="126" spans="2:13" ht="15">
       <c r="B126" s="38"/>
-      <c r="F126" s="11"/>
-    </row>
-    <row r="127" spans="2:7" ht="15">
+      <c r="C126" s="24"/>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4"/>
+    </row>
+    <row r="127" spans="2:13" ht="15">
       <c r="B127" s="38"/>
-    </row>
-    <row r="128" spans="2:7" ht="15">
+      <c r="G127" s="4"/>
+    </row>
+    <row r="128" spans="2:13" ht="15">
       <c r="B128" s="38"/>
+      <c r="F128" s="11"/>
     </row>
     <row r="129" spans="2:8" ht="15">
       <c r="B129" s="38"/>
-      <c r="F129" s="4"/>
-      <c r="G129" s="4"/>
     </row>
     <row r="130" spans="2:8" ht="15">
       <c r="B130" s="38"/>
-      <c r="F130" s="11"/>
-      <c r="G130" s="4"/>
     </row>
     <row r="131" spans="2:8" ht="15">
       <c r="B131" s="38"/>
-      <c r="F131" s="11"/>
-      <c r="G131" s="11"/>
+      <c r="F131" s="4"/>
+      <c r="G131" s="4"/>
     </row>
     <row r="132" spans="2:8" ht="15">
+      <c r="B132" s="38"/>
+      <c r="F132" s="11"/>
       <c r="G132" s="4"/>
     </row>
-    <row r="136" spans="2:8" ht="15">
-      <c r="B136" s="109"/>
-      <c r="C136" s="109"/>
-    </row>
-    <row r="137" spans="2:8" ht="15">
-      <c r="F137" s="11"/>
-      <c r="H137" s="39"/>
+    <row r="133" spans="2:8" ht="15">
+      <c r="B133" s="38"/>
+      <c r="F133" s="11"/>
+      <c r="G133" s="11"/>
+    </row>
+    <row r="134" spans="2:8" ht="15">
+      <c r="G134" s="4"/>
     </row>
     <row r="138" spans="2:8" ht="15">
-      <c r="H138" s="39"/>
+      <c r="B138" s="96"/>
+      <c r="C138" s="96"/>
     </row>
     <row r="139" spans="2:8" ht="15">
+      <c r="F139" s="11"/>
       <c r="H139" s="39"/>
     </row>
     <row r="140" spans="2:8" ht="15">
@@ -3332,17 +3360,11 @@
     <row r="148" spans="8:14" ht="15">
       <c r="H148" s="39"/>
     </row>
+    <row r="149" spans="8:14" ht="15">
+      <c r="H149" s="39"/>
+    </row>
     <row r="150" spans="8:14" ht="15">
-      <c r="I150" s="38"/>
-      <c r="J150" s="2"/>
-      <c r="L150" s="40"/>
-      <c r="M150" s="40"/>
-    </row>
-    <row r="151" spans="8:14" ht="15">
-      <c r="I151" s="38"/>
-      <c r="J151" s="2"/>
-      <c r="L151" s="40"/>
-      <c r="M151" s="40"/>
+      <c r="H150" s="39"/>
     </row>
     <row r="152" spans="8:14" ht="15">
       <c r="I152" s="38"/>
@@ -3358,21 +3380,21 @@
     </row>
     <row r="154" spans="8:14" ht="15">
       <c r="I154" s="38"/>
+      <c r="J154" s="2"/>
+      <c r="L154" s="40"/>
+      <c r="M154" s="40"/>
     </row>
     <row r="155" spans="8:14" ht="15">
       <c r="I155" s="38"/>
-      <c r="N155" s="11"/>
+      <c r="J155" s="2"/>
+      <c r="L155" s="40"/>
+      <c r="M155" s="40"/>
     </row>
     <row r="156" spans="8:14" ht="15">
       <c r="I156" s="38"/>
-      <c r="L156" s="40"/>
-      <c r="M156" s="40"/>
-      <c r="N156" s="11"/>
     </row>
     <row r="157" spans="8:14" ht="15">
       <c r="I157" s="38"/>
-      <c r="L157" s="40"/>
-      <c r="M157" s="40"/>
       <c r="N157" s="11"/>
     </row>
     <row r="158" spans="8:14" ht="15">
@@ -3383,6 +3405,8 @@
     </row>
     <row r="159" spans="8:14" ht="15">
       <c r="I159" s="38"/>
+      <c r="L159" s="40"/>
+      <c r="M159" s="40"/>
       <c r="N159" s="11"/>
     </row>
     <row r="160" spans="8:14" ht="15">
@@ -3403,8 +3427,6 @@
     </row>
     <row r="163" spans="3:14" ht="15">
       <c r="I163" s="38"/>
-      <c r="L163" s="40"/>
-      <c r="M163" s="40"/>
       <c r="N163" s="11"/>
     </row>
     <row r="164" spans="3:14" ht="15">
@@ -3415,43 +3437,55 @@
     </row>
     <row r="165" spans="3:14" ht="15">
       <c r="I165" s="38"/>
+      <c r="L165" s="40"/>
+      <c r="M165" s="40"/>
+      <c r="N165" s="11"/>
     </row>
     <row r="166" spans="3:14" ht="15">
       <c r="I166" s="38"/>
+      <c r="L166" s="40"/>
+      <c r="M166" s="40"/>
+      <c r="N166" s="11"/>
     </row>
     <row r="167" spans="3:14" ht="15">
       <c r="I167" s="38"/>
     </row>
     <row r="168" spans="3:14" ht="15">
-      <c r="I168" s="41"/>
+      <c r="I168" s="38"/>
     </row>
     <row r="169" spans="3:14" ht="15">
-      <c r="F169" s="11"/>
       <c r="I169" s="38"/>
-      <c r="N169" s="11"/>
     </row>
     <row r="170" spans="3:14" ht="15">
-      <c r="C170" s="37"/>
-      <c r="D170" s="37"/>
-      <c r="F170" s="11"/>
-      <c r="I170" s="38"/>
+      <c r="I170" s="41"/>
     </row>
     <row r="171" spans="3:14" ht="15">
+      <c r="F171" s="11"/>
       <c r="I171" s="38"/>
       <c r="N171" s="11"/>
     </row>
     <row r="172" spans="3:14" ht="15">
+      <c r="C172" s="37"/>
+      <c r="D172" s="37"/>
+      <c r="F172" s="11"/>
       <c r="I172" s="38"/>
-      <c r="N172" s="11"/>
     </row>
     <row r="173" spans="3:14" ht="15">
       <c r="I173" s="38"/>
       <c r="N173" s="11"/>
     </row>
+    <row r="174" spans="3:14" ht="15">
+      <c r="I174" s="38"/>
+      <c r="N174" s="11"/>
+    </row>
+    <row r="175" spans="3:14" ht="15">
+      <c r="I175" s="38"/>
+      <c r="N175" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B138:C138"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39375000000000004" bottom="0.39375000000000004" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3464,57 +3498,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:O53"/>
+  <dimension ref="B1:O56"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.5" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="42" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="42" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="1.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" style="2"/>
-    <col min="12" max="12" width="14.1640625" style="95"/>
+    <col min="11" max="11" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="82" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="1.5" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="14.1640625" style="2"/>
+    <col min="14" max="14" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="14.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="6" customHeight="1"/>
     <row r="2" spans="2:15" ht="20">
       <c r="B2" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="6" customHeight="1"/>
     <row r="4" spans="2:15" ht="16">
       <c r="B4" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="I4" s="97"/>
+      <c r="K4" s="97" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="110" t="s">
+      <c r="L4" s="97"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="97" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="110"/>
-      <c r="K4" s="110" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" s="110"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="110" t="s">
-        <v>96</v>
-      </c>
-      <c r="O4" s="110"/>
+      <c r="O4" s="97"/>
     </row>
     <row r="5" spans="2:15" ht="6" customHeight="1">
       <c r="B5" s="46"/>
@@ -3523,495 +3559,616 @@
       <c r="F5" s="47"/>
     </row>
     <row r="6" spans="2:15" ht="14">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="E6" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="H6" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="51"/>
+      <c r="K6" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="E6" s="50" t="s">
+      <c r="L6" s="87"/>
+      <c r="N6" s="104" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="H6" s="52" t="s">
+      <c r="O6" s="105"/>
+    </row>
+    <row r="7" spans="2:15" ht="14">
+      <c r="B7" s="62"/>
+      <c r="C7" s="57"/>
+      <c r="E7" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="53"/>
-      <c r="K6" s="99" t="s">
+      <c r="F7" s="49">
+        <v>452</v>
+      </c>
+      <c r="H7" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="100"/>
-      <c r="N6" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="O6" s="55"/>
-    </row>
-    <row r="7" spans="2:15" ht="14">
-      <c r="B7" s="56" t="s">
+      <c r="I7" s="51">
+        <v>340.91</v>
+      </c>
+      <c r="K7" s="88"/>
+      <c r="L7" s="89"/>
+      <c r="N7" s="106" t="s">
         <v>102</v>
       </c>
-      <c r="C7" s="57">
-        <v>17600</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="51">
-        <v>452</v>
-      </c>
-      <c r="H7" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" s="53">
-        <v>340.91</v>
-      </c>
-      <c r="K7" s="101"/>
-      <c r="L7" s="102"/>
-      <c r="N7" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="O7" s="55">
+      <c r="O7" s="105">
         <f>286+70</f>
         <v>356</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="14">
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="57">
+        <v>250</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="49">
+        <v>1023</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="51">
+        <v>100</v>
+      </c>
+      <c r="K8" s="88" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="89">
+        <v>296</v>
+      </c>
+      <c r="N8" s="106" t="s">
+        <v>105</v>
+      </c>
+      <c r="O8" s="105">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="14">
+      <c r="B9" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="57">
+        <v>120</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="49">
+        <v>500</v>
+      </c>
+      <c r="H9" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="57">
-        <v>20000</v>
-      </c>
-      <c r="E8" s="58" t="s">
+      <c r="I9" s="51">
+        <v>170</v>
+      </c>
+      <c r="K9" s="88" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="89">
+        <v>1100</v>
+      </c>
+      <c r="N9" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="O9" s="105">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="14">
+      <c r="B10" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="57">
+        <v>85</v>
+      </c>
+      <c r="E10" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="F8" s="51">
-        <v>1023</v>
-      </c>
-      <c r="H8" s="59" t="s">
+      <c r="F10" s="49">
+        <v>100</v>
+      </c>
+      <c r="H10" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="53">
-        <v>100</v>
-      </c>
-      <c r="K8" s="101" t="s">
-        <v>105</v>
-      </c>
-      <c r="L8" s="102">
-        <v>296</v>
-      </c>
-      <c r="N8" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="O8" s="55">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="14">
-      <c r="B9" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="57">
-        <v>20000</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="51">
-        <v>500</v>
-      </c>
-      <c r="H9" s="59" t="s">
-        <v>113</v>
-      </c>
-      <c r="I9" s="53">
-        <v>170</v>
-      </c>
-      <c r="K9" s="101" t="s">
-        <v>147</v>
-      </c>
-      <c r="L9" s="102">
-        <v>1100</v>
-      </c>
-      <c r="N9" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="O9" s="55">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="14">
-      <c r="B10" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="57">
-        <v>20000</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="51">
-        <v>100</v>
-      </c>
-      <c r="H10" s="59" t="s">
-        <v>117</v>
-      </c>
-      <c r="I10" s="53">
+      <c r="I10" s="51">
         <v>150</v>
       </c>
-      <c r="K10" s="101" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" s="102">
+      <c r="K10" s="88" t="s">
+        <v>99</v>
+      </c>
+      <c r="L10" s="89">
         <v>532</v>
       </c>
-      <c r="N10" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="O10" s="61">
+      <c r="N10" s="104" t="s">
+        <v>163</v>
+      </c>
+      <c r="O10" s="107">
         <f>SUM(O7:O9)</f>
         <v>676</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="14">
-      <c r="B11" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="62">
-        <f>SUM(C7:C10)</f>
-        <v>77600</v>
-      </c>
-      <c r="E11" s="50" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" s="63">
+      <c r="B11" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="57">
+        <v>150</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="54">
         <f>SUM(F7:F10)</f>
         <v>2075</v>
       </c>
-      <c r="H11" s="52" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="64">
+      <c r="H11" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="55">
         <f>SUM(I7:I10)</f>
         <v>760.91000000000008</v>
       </c>
-      <c r="K11" s="101" t="s">
+      <c r="K11" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="L11" s="102">
-        <f>3000-3*SUM(C16:C17)</f>
-        <v>2385</v>
+      <c r="L11" s="89">
+        <f>3000-3*SUM(C8:C9)</f>
+        <v>1890</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="14">
+      <c r="B12" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="66">
+        <f>SUM(C6:C11)</f>
+        <v>605</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="F12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="K12" s="101" t="s">
+      <c r="K12" s="88" t="s">
+        <v>111</v>
+      </c>
+      <c r="L12" s="89">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="14">
+      <c r="D13" s="4"/>
+      <c r="E13" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="59"/>
+      <c r="H13" s="60" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="61"/>
+      <c r="K13" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="89">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="14">
+      <c r="B14" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="69"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="59">
+        <v>350</v>
+      </c>
+      <c r="H14" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" s="61">
+        <v>175</v>
+      </c>
+      <c r="K14" s="88"/>
+      <c r="L14" s="89"/>
+    </row>
+    <row r="15" spans="2:15" ht="14">
+      <c r="B15" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="69">
+        <v>156</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="59">
+        <v>1287</v>
+      </c>
+      <c r="H15" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="61">
+        <v>163</v>
+      </c>
+      <c r="K15" s="86" t="s">
+        <v>110</v>
+      </c>
+      <c r="L15" s="89">
+        <f>SUM(L8:L14)</f>
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="14">
+      <c r="B16" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="69">
+        <v>20</v>
+      </c>
+      <c r="E16" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="L12" s="102">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="14">
-      <c r="B13" s="65" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="67" t="s">
+      <c r="F16" s="59">
+        <v>650</v>
+      </c>
+      <c r="H16" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="61">
+        <v>480</v>
+      </c>
+      <c r="L16" s="42"/>
+    </row>
+    <row r="17" spans="2:15" ht="14">
+      <c r="B17" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="74">
+        <f>SUM(C15:C16)</f>
+        <v>176</v>
+      </c>
+      <c r="E17" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="68"/>
-      <c r="H13" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="I13" s="70"/>
-      <c r="K13" s="101" t="s">
-        <v>148</v>
-      </c>
-      <c r="L13" s="102">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="14">
-      <c r="B14" s="71"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="68">
-        <v>350</v>
-      </c>
-      <c r="H14" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="I14" s="70">
-        <v>175</v>
-      </c>
-      <c r="K14" s="101"/>
-      <c r="L14" s="102"/>
-    </row>
-    <row r="15" spans="2:15" ht="14">
-      <c r="B15" s="71" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="66">
-        <v>250</v>
-      </c>
-      <c r="E15" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="F15" s="68">
-        <v>1287</v>
-      </c>
-      <c r="H15" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="I15" s="70">
-        <v>163</v>
-      </c>
-      <c r="K15" s="99" t="s">
-        <v>118</v>
-      </c>
-      <c r="L15" s="102">
-        <f>SUM(L8:L14)</f>
-        <v>4905</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="14">
-      <c r="B16" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="66">
-        <v>120</v>
-      </c>
-      <c r="E16" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="F16" s="68">
-        <v>650</v>
-      </c>
-      <c r="H16" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="70">
-        <v>480</v>
-      </c>
-      <c r="L16" s="42"/>
-    </row>
-    <row r="17" spans="2:12" ht="14">
-      <c r="B17" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="66">
-        <v>85</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="F17" s="68">
+      <c r="F17" s="59">
         <v>750</v>
       </c>
-      <c r="H17" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="74">
+      <c r="H17" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" s="65">
         <f>SUM(I14:I16)</f>
         <v>818</v>
       </c>
-      <c r="K17" s="96" t="s">
-        <v>162</v>
-      </c>
-      <c r="L17" s="98"/>
-    </row>
-    <row r="18" spans="2:12" ht="14">
-      <c r="B18" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="66">
-        <v>150</v>
-      </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="68"/>
-      <c r="K18" s="97"/>
-      <c r="L18" s="98"/>
-    </row>
-    <row r="19" spans="2:12" ht="14">
-      <c r="B19" s="65" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="75">
-        <f>SUM(C13:C18)</f>
-        <v>605</v>
-      </c>
-      <c r="E19" s="67" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" s="76">
+      <c r="K17" s="110" t="s">
+        <v>168</v>
+      </c>
+      <c r="L17" s="109"/>
+    </row>
+    <row r="18" spans="2:15" ht="14">
+      <c r="E18" s="63"/>
+      <c r="F18" s="59"/>
+      <c r="K18" s="111" t="s">
+        <v>99</v>
+      </c>
+      <c r="L18" s="112">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="14">
+      <c r="E19" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="67">
         <f>SUM(F14:F18)</f>
         <v>3037</v>
       </c>
-      <c r="H19" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="I19" s="78"/>
-      <c r="K19" s="97" t="s">
-        <v>147</v>
-      </c>
-      <c r="L19" s="98">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" ht="14">
+      <c r="H19" s="100" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="101"/>
+      <c r="K19" s="111" t="s">
+        <v>161</v>
+      </c>
+      <c r="L19" s="112">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="14">
       <c r="F20" s="2"/>
-      <c r="H20" s="79" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="78">
+      <c r="H20" s="102" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20" s="101">
         <v>31</v>
       </c>
-      <c r="K20" s="97" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="98">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" ht="14">
-      <c r="B21" s="80" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="81"/>
-      <c r="E21" s="82" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="83"/>
-      <c r="H21" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="78">
+      <c r="K20" s="111" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="112">
+        <f>2000-2*SUM(C32:C33)</f>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="14">
+      <c r="E21" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" s="71"/>
+      <c r="H21" s="102" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" s="101">
         <v>553</v>
       </c>
-      <c r="K21" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="L21" s="98">
-        <f>3000-3*SUM(C17:C18)</f>
-        <v>2295</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="14">
-      <c r="B22" s="84" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="81">
-        <v>156</v>
-      </c>
-      <c r="E22" s="83" t="s">
-        <v>135</v>
-      </c>
-      <c r="F22" s="83">
+      <c r="K21" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="L21" s="112">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="14">
+      <c r="E22" s="71" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="71">
         <f>F11</f>
         <v>2075</v>
       </c>
-      <c r="H22" s="79" t="s">
-        <v>109</v>
-      </c>
-      <c r="I22" s="78">
+      <c r="H22" s="102" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" s="101">
         <v>35</v>
       </c>
-      <c r="K22" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="L22" s="98">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="14">
-      <c r="B23" s="84" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="81">
-        <v>20</v>
-      </c>
-      <c r="E23" s="83" t="s">
-        <v>121</v>
-      </c>
-      <c r="F23" s="83">
+      <c r="K22" s="111" t="s">
+        <v>111</v>
+      </c>
+      <c r="L22" s="112">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="14">
+      <c r="E23" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="71">
         <f>F19</f>
         <v>3037</v>
       </c>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="78">
+      <c r="I23" s="101">
         <v>280</v>
       </c>
-      <c r="K23" s="96"/>
-      <c r="L23" s="103"/>
-    </row>
-    <row r="24" spans="2:12" ht="14">
-      <c r="B24" s="85" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="86">
-        <f>SUM(C22:C23)</f>
-        <v>176</v>
-      </c>
-      <c r="E24" s="82" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="82">
+      <c r="K23" s="108"/>
+      <c r="L23" s="109"/>
+    </row>
+    <row r="24" spans="2:15" ht="14">
+      <c r="E24" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="70">
         <f>SUM(F22:F23)</f>
         <v>5112</v>
       </c>
-      <c r="H24" s="77" t="s">
-        <v>118</v>
-      </c>
-      <c r="I24" s="87">
+      <c r="H24" s="100" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="103">
         <f>SUM(I20:I23)</f>
         <v>899</v>
       </c>
-      <c r="K24" s="96" t="s">
+      <c r="K24" s="110" t="s">
+        <v>110</v>
+      </c>
+      <c r="L24" s="113">
+        <f>SUM(L18:L23)</f>
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="14">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:15" ht="20">
+      <c r="B26" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="6" customHeight="1"/>
+    <row r="28" spans="2:15" ht="16">
+      <c r="B28" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="I28" s="97"/>
+      <c r="K28" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="L28" s="97"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="O28" s="97"/>
+    </row>
+    <row r="29" spans="2:15" ht="6" customHeight="1">
+      <c r="B29" s="46"/>
+      <c r="C29" s="47"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="47"/>
+    </row>
+    <row r="30" spans="2:15" ht="14">
+      <c r="B30" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="57"/>
+      <c r="E30" s="83" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" s="85"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="2:15" ht="14">
+      <c r="B31" s="62"/>
+      <c r="C31" s="57"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="85"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="2:15" ht="14">
+      <c r="B32" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="57">
+        <v>250</v>
+      </c>
+      <c r="E32" s="84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="85">
+        <v>1500</v>
+      </c>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="2:9" ht="14">
+      <c r="B33" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="L24" s="103">
-        <f>SUM(L20:L23)</f>
-        <v>2745</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="14">
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="2:12" ht="14">
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="2:12" ht="14">
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="2:12" ht="14">
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="2:12" ht="14">
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="2:12" ht="14">
-      <c r="I30" s="2"/>
-    </row>
-    <row r="40" spans="6:6" ht="14">
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="6:6" ht="14">
-      <c r="F41" s="2"/>
-    </row>
-    <row r="53" spans="3:3" ht="14">
-      <c r="C53" s="88"/>
+      <c r="C33" s="57">
+        <v>120</v>
+      </c>
+      <c r="E33" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" s="85">
+        <v>200</v>
+      </c>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B34" s="62" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" s="57">
+        <f>20+50+42</f>
+        <v>112</v>
+      </c>
+      <c r="E34" s="84" t="s">
+        <v>127</v>
+      </c>
+      <c r="F34" s="85">
+        <f>3000-3*SUM(C32:C33)</f>
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B35" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" s="57">
+        <v>150</v>
+      </c>
+      <c r="E35" s="84" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="85">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B36" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="66">
+        <f>SUM(C30:C35)</f>
+        <v>632</v>
+      </c>
+      <c r="E36" s="83"/>
+      <c r="F36" s="90"/>
+    </row>
+    <row r="37" spans="2:9" ht="13.5" customHeight="1">
+      <c r="E37" s="83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="90">
+        <f>SUM(F32:F36)</f>
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B38" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="69"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B39" s="72" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="69">
+        <v>156</v>
+      </c>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B40" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="13.5" customHeight="1">
+      <c r="B41" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="74">
+        <f>SUM(C39:C40)</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="14">
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="2:9" ht="14">
+      <c r="F44" s="2"/>
+    </row>
+    <row r="56" spans="3:3" ht="14">
+      <c r="C56" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="N28:O28"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39375000000000004" bottom="0.39375000000000004" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>